<commit_message>
added sprint 2 backlog items
</commit_message>
<xml_diff>
--- a/Documentation/backlogs/masterProductBacklog.xlsx
+++ b/Documentation/backlogs/masterProductBacklog.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="74" uniqueCount="41">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="150" uniqueCount="75">
   <si>
     <t>Sprints</t>
   </si>
@@ -132,9 +132,6 @@
     <t>Sprint 5</t>
   </si>
   <si>
-    <t>Priority  (high = 1)</t>
-  </si>
-  <si>
     <t>Sprint 4 Backlog</t>
   </si>
   <si>
@@ -142,13 +139,119 @@
   </si>
   <si>
     <t>Product and Sprint Backlog with Summaries</t>
+  </si>
+  <si>
+    <t>Allow user to make appointments</t>
+  </si>
+  <si>
+    <t>Email ICS Calendar invitation</t>
+  </si>
+  <si>
+    <t>Retrieve Faculty list from Café</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Retrieve faculty office hours from Café </t>
+  </si>
+  <si>
+    <t>Display calendar on webpage</t>
+  </si>
+  <si>
+    <t>Authenticate / Identify user</t>
+  </si>
+  <si>
+    <t>Define Appointment database schema</t>
+  </si>
+  <si>
+    <t>General Web UI</t>
+  </si>
+  <si>
+    <t>Priority  (high = 1 / 5 = low)</t>
+  </si>
+  <si>
+    <t>Define what new databases we need for the program</t>
+  </si>
+  <si>
+    <t>Define overall database structure, accounting for what data is available and what data we need from the Cafe system.</t>
+  </si>
+  <si>
+    <t>Create any new databases and/or tables in microsoft sql on our project side (ie. not in cafe)</t>
+  </si>
+  <si>
+    <t>Test cases: What is the form of the data for each record; How is it validated</t>
+  </si>
+  <si>
+    <t>Naif</t>
+  </si>
+  <si>
+    <t>Define the format of the ICS file/files we need for the project</t>
+  </si>
+  <si>
+    <t>Send a calendar file</t>
+  </si>
+  <si>
+    <t>Validate working with Gannon outlook</t>
+  </si>
+  <si>
+    <t>Validate accept/decline uses</t>
+  </si>
+  <si>
+    <t>Define best user flow for sending receiving</t>
+  </si>
+  <si>
+    <t>What data do we need from user / prof to send receive invites</t>
+  </si>
+  <si>
+    <t>Jimmy</t>
+  </si>
+  <si>
+    <t>Investigate its ability to be extended to include visual indication of: Professors’ Office Hours; Current appointments</t>
+  </si>
+  <si>
+    <t>Create Basic calendar in C# / ASP.NET that can be used/migrated to a webapp in those technologies</t>
+  </si>
+  <si>
+    <t>Andrew</t>
+  </si>
+  <si>
+    <t>Retrieve data from Cafe system</t>
+  </si>
+  <si>
+    <t>Define the interface between our system (dbs, controller logic) and the cafe system (specifically, its data)</t>
+  </si>
+  <si>
+    <t>Tom</t>
+  </si>
+  <si>
+    <t>In Progress</t>
+  </si>
+  <si>
+    <t>Completed</t>
+  </si>
+  <si>
+    <t>Each member creates his own set of perceived project features and subtasks.</t>
+  </si>
+  <si>
+    <t>Each member estimates priority and difficulty of main features and subtasks</t>
+  </si>
+  <si>
+    <t>Each member learns unknown technologies
+ C#, ASP.NET, SQL, Git</t>
+  </si>
+  <si>
+    <t>*</t>
+  </si>
+  <si>
+    <t>All</t>
+  </si>
+  <si>
+    <t>Create Preliminary Product Backlog and System Diagrams</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="10" x14ac:knownFonts="1">
+  <fonts count="11" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -219,6 +322,12 @@
       <name val="Times New Roman"/>
       <family val="1"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
   </fonts>
   <fills count="3">
     <fill>
@@ -250,7 +359,7 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="39">
+  <cellXfs count="46">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -281,9 +390,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="14" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -301,9 +407,6 @@
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="16" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -340,6 +443,12 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -357,6 +466,25 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" indent="4"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="6">
@@ -702,16 +830,16 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G75"/>
+  <dimension ref="A1:G89"/>
   <sheetViews>
     <sheetView tabSelected="1" showRuler="0" zoomScale="78" zoomScaleNormal="78" workbookViewId="0">
-      <selection activeCell="E4" sqref="E4:E5"/>
+      <selection activeCell="C7" sqref="C7:E7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.125" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="6.5" customWidth="1"/>
-    <col min="2" max="2" width="51.375" style="14" customWidth="1"/>
+    <col min="2" max="2" width="51.375" style="13" customWidth="1"/>
     <col min="3" max="3" width="34.375" customWidth="1"/>
     <col min="4" max="4" width="23.75" customWidth="1"/>
     <col min="5" max="5" width="26.5" customWidth="1"/>
@@ -721,70 +849,76 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:6" ht="18" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="21"/>
-      <c r="B1" s="23" t="s">
+      <c r="A1" s="19"/>
+      <c r="B1" s="21" t="s">
         <v>33</v>
       </c>
       <c r="C1" s="33" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="D1" s="33"/>
       <c r="E1" s="33"/>
-      <c r="F1" s="22" t="s">
+      <c r="F1" s="20" t="s">
         <v>35</v>
       </c>
     </row>
     <row r="2" spans="1:6" ht="18" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="22"/>
-      <c r="B2" s="22" t="s">
+      <c r="A2" s="20"/>
+      <c r="B2" s="20" t="s">
         <v>34</v>
       </c>
       <c r="C2" s="34"/>
       <c r="D2" s="34"/>
       <c r="E2" s="34"/>
-      <c r="F2" s="22"/>
+      <c r="F2" s="20"/>
     </row>
     <row r="3" spans="1:6" ht="18" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="22"/>
+      <c r="A3" s="20"/>
       <c r="B3" s="36"/>
-      <c r="C3" s="25" t="s">
+      <c r="C3" s="23" t="s">
         <v>25</v>
       </c>
-      <c r="D3" s="25" t="s">
+      <c r="D3" s="23" t="s">
         <v>26</v>
       </c>
-      <c r="E3" s="24"/>
-      <c r="F3" s="22"/>
+      <c r="E3" s="22"/>
+      <c r="F3" s="20"/>
     </row>
     <row r="4" spans="1:6" ht="18" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A4" s="22"/>
+      <c r="A4" s="20"/>
       <c r="B4" s="36"/>
-      <c r="C4" s="24" t="s">
+      <c r="C4" s="22" t="s">
         <v>28</v>
       </c>
-      <c r="D4" s="26"/>
-      <c r="E4" s="24"/>
-      <c r="F4" s="22"/>
+      <c r="D4" s="24">
+        <v>42463</v>
+      </c>
+      <c r="E4" s="22"/>
+      <c r="F4" s="20"/>
     </row>
     <row r="5" spans="1:6" ht="18" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A5" s="22"/>
+      <c r="A5" s="20"/>
       <c r="B5" s="36"/>
-      <c r="C5" s="24" t="s">
+      <c r="C5" s="22" t="s">
         <v>29</v>
       </c>
-      <c r="D5" s="26"/>
-      <c r="E5" s="24"/>
-      <c r="F5" s="22"/>
+      <c r="D5" s="24">
+        <v>42463</v>
+      </c>
+      <c r="E5" s="22"/>
+      <c r="F5" s="20"/>
     </row>
     <row r="6" spans="1:6" ht="18" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A6" s="22"/>
+      <c r="A6" s="20"/>
       <c r="B6" s="36"/>
-      <c r="C6" s="24" t="s">
+      <c r="C6" s="22" t="s">
         <v>24</v>
       </c>
-      <c r="D6" s="26"/>
-      <c r="E6" s="24"/>
-      <c r="F6" s="22"/>
+      <c r="D6" s="24">
+        <v>42467</v>
+      </c>
+      <c r="E6" s="22"/>
+      <c r="F6" s="20"/>
     </row>
     <row r="7" spans="1:6" ht="18" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A7" s="2"/>
@@ -802,7 +936,7 @@
       <c r="A9" s="7" t="s">
         <v>1</v>
       </c>
-      <c r="B9" s="15" t="s">
+      <c r="B9" s="14" t="s">
         <v>2</v>
       </c>
       <c r="C9" s="7" t="s">
@@ -825,9 +959,15 @@
       <c r="B10" s="5" t="s">
         <v>6</v>
       </c>
-      <c r="C10" s="4"/>
-      <c r="D10" s="4"/>
-      <c r="E10" s="3"/>
+      <c r="C10" s="4">
+        <v>42451</v>
+      </c>
+      <c r="D10" s="4">
+        <v>42465</v>
+      </c>
+      <c r="E10" s="3" t="s">
+        <v>68</v>
+      </c>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A11" s="1">
@@ -836,9 +976,15 @@
       <c r="B11" s="5" t="s">
         <v>7</v>
       </c>
-      <c r="C11" s="12"/>
-      <c r="D11" s="4"/>
-      <c r="E11" s="13"/>
+      <c r="C11" s="4">
+        <v>42465</v>
+      </c>
+      <c r="D11" s="4">
+        <v>42472</v>
+      </c>
+      <c r="E11" s="3" t="s">
+        <v>67</v>
+      </c>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A12" s="1">
@@ -847,38 +993,50 @@
       <c r="B12" s="10" t="s">
         <v>11</v>
       </c>
-      <c r="C12" s="17"/>
-      <c r="D12" s="17"/>
-      <c r="E12" s="13"/>
+      <c r="C12" s="16">
+        <v>42472</v>
+      </c>
+      <c r="D12" s="16">
+        <v>42479</v>
+      </c>
+      <c r="E12" s="12"/>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A13" s="1">
         <v>4</v>
       </c>
-      <c r="B13" s="31" t="s">
+      <c r="B13" s="29" t="s">
         <v>31</v>
       </c>
-      <c r="C13" s="17"/>
-      <c r="D13" s="17"/>
-      <c r="E13" s="13"/>
+      <c r="C13" s="16">
+        <v>42479</v>
+      </c>
+      <c r="D13" s="16">
+        <v>42486</v>
+      </c>
+      <c r="E13" s="12"/>
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A14" s="1">
         <v>5</v>
       </c>
-      <c r="B14" s="31" t="s">
+      <c r="B14" s="29" t="s">
         <v>36</v>
       </c>
-      <c r="C14" s="17"/>
-      <c r="D14" s="17"/>
-      <c r="E14" s="13"/>
+      <c r="C14" s="16">
+        <v>42486</v>
+      </c>
+      <c r="D14" s="16">
+        <v>42490</v>
+      </c>
+      <c r="E14" s="12"/>
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A15" s="1"/>
-      <c r="B15" s="31"/>
-      <c r="C15" s="17"/>
-      <c r="D15" s="17"/>
-      <c r="E15" s="13"/>
+      <c r="B15" s="29"/>
+      <c r="C15" s="16"/>
+      <c r="D15" s="16"/>
+      <c r="E15" s="12"/>
     </row>
     <row r="16" spans="1:6" ht="15.6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A16" s="2"/>
@@ -887,19 +1045,19 @@
       <c r="B17" s="6" t="s">
         <v>8</v>
       </c>
-      <c r="C17" s="18" t="s">
+      <c r="C17" s="17" t="s">
         <v>32</v>
       </c>
-      <c r="D17" s="18" t="s">
+      <c r="D17" s="17" t="s">
         <v>6</v>
       </c>
-      <c r="E17" s="18" t="s">
+      <c r="E17" s="17" t="s">
         <v>7</v>
       </c>
-      <c r="F17" s="18" t="s">
+      <c r="F17" s="17" t="s">
         <v>21</v>
       </c>
-      <c r="G17" s="18" t="s">
+      <c r="G17" s="17" t="s">
         <v>31</v>
       </c>
     </row>
@@ -907,11 +1065,11 @@
       <c r="A18" s="7" t="s">
         <v>1</v>
       </c>
-      <c r="B18" s="15" t="s">
-        <v>37</v>
-      </c>
-      <c r="C18" s="7" t="s">
+      <c r="B18" s="14" t="s">
         <v>17</v>
+      </c>
+      <c r="C18" s="14" t="s">
+        <v>48</v>
       </c>
       <c r="D18" s="8" t="s">
         <v>18</v>
@@ -930,9 +1088,16 @@
       <c r="A19" s="1">
         <v>0</v>
       </c>
-      <c r="B19" s="10"/>
+      <c r="B19" s="10" t="s">
+        <v>40</v>
+      </c>
+      <c r="C19">
+        <v>1</v>
+      </c>
       <c r="D19" s="1"/>
-      <c r="E19" s="1"/>
+      <c r="E19" s="1" t="s">
+        <v>67</v>
+      </c>
       <c r="F19" s="1"/>
       <c r="G19" s="1"/>
     </row>
@@ -940,110 +1105,152 @@
       <c r="A20" s="1">
         <v>1</v>
       </c>
-      <c r="B20" s="5"/>
-      <c r="C20" s="3"/>
+      <c r="B20" s="5" t="s">
+        <v>41</v>
+      </c>
+      <c r="C20" s="3">
+        <v>2</v>
+      </c>
       <c r="D20" s="1"/>
-      <c r="E20" s="3"/>
-      <c r="F20" s="29"/>
+      <c r="E20" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="F20" s="27"/>
       <c r="G20" s="1"/>
     </row>
     <row r="21" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A21" s="27">
+      <c r="A21" s="25">
         <v>2</v>
       </c>
-      <c r="B21" s="30"/>
-      <c r="C21" s="20"/>
-      <c r="D21" s="27"/>
-      <c r="E21" s="20"/>
-      <c r="F21" s="32"/>
+      <c r="B21" s="28" t="s">
+        <v>42</v>
+      </c>
+      <c r="C21" s="18">
+        <v>2</v>
+      </c>
+      <c r="D21" s="25"/>
+      <c r="E21" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="F21" s="30"/>
       <c r="G21" s="1"/>
     </row>
     <row r="22" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A22" s="27">
+      <c r="A22" s="25">
         <v>3</v>
       </c>
-      <c r="B22" s="5"/>
-      <c r="C22" s="20"/>
+      <c r="B22" s="5" t="s">
+        <v>43</v>
+      </c>
+      <c r="C22" s="18">
+        <v>1</v>
+      </c>
       <c r="D22" s="1"/>
-      <c r="E22" s="3"/>
-      <c r="F22" s="29"/>
+      <c r="E22" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="F22" s="27"/>
       <c r="G22" s="1"/>
     </row>
     <row r="23" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A23" s="27">
+      <c r="A23" s="25">
         <v>4</v>
       </c>
-      <c r="B23" s="5"/>
-      <c r="C23" s="20"/>
+      <c r="B23" s="5" t="s">
+        <v>44</v>
+      </c>
+      <c r="C23" s="18">
+        <v>3</v>
+      </c>
       <c r="D23" s="1"/>
-      <c r="E23" s="3"/>
-      <c r="F23" s="29"/>
+      <c r="E23" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="F23" s="27"/>
       <c r="G23" s="1"/>
     </row>
     <row r="24" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A24" s="27">
+      <c r="A24" s="25">
         <v>5</v>
       </c>
-      <c r="B24" s="30"/>
-      <c r="C24" s="20"/>
-      <c r="D24" s="27"/>
-      <c r="E24" s="20"/>
-      <c r="F24" s="32"/>
+      <c r="B24" s="28" t="s">
+        <v>45</v>
+      </c>
+      <c r="C24" s="18">
+        <v>4</v>
+      </c>
+      <c r="D24" s="25"/>
+      <c r="E24" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="F24" s="30"/>
       <c r="G24" s="1"/>
     </row>
     <row r="25" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A25" s="27">
+      <c r="A25" s="25">
         <v>6</v>
       </c>
-      <c r="B25" s="5"/>
-      <c r="C25" s="3"/>
+      <c r="B25" s="5" t="s">
+        <v>46</v>
+      </c>
+      <c r="C25" s="3">
+        <v>1</v>
+      </c>
       <c r="D25" s="1"/>
-      <c r="E25" s="3"/>
-      <c r="F25" s="29"/>
+      <c r="E25" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="F25" s="27"/>
       <c r="G25" s="1"/>
     </row>
     <row r="26" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A26" s="27">
+      <c r="A26" s="25">
         <v>7</v>
       </c>
-      <c r="B26" s="5"/>
-      <c r="C26" s="20"/>
+      <c r="B26" s="5" t="s">
+        <v>47</v>
+      </c>
+      <c r="C26" s="18">
+        <v>3</v>
+      </c>
       <c r="D26" s="1"/>
-      <c r="E26" s="3"/>
-      <c r="F26" s="29"/>
+      <c r="E26" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="F26" s="27"/>
       <c r="G26" s="1"/>
     </row>
     <row r="27" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A27" s="27">
+      <c r="A27" s="25">
         <v>8</v>
       </c>
       <c r="B27" s="10"/>
       <c r="C27" s="1"/>
       <c r="D27" s="10"/>
       <c r="E27" s="3"/>
-      <c r="F27" s="29"/>
+      <c r="F27" s="27"/>
       <c r="G27" s="1"/>
     </row>
     <row r="28" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A28" s="27">
+      <c r="A28" s="25">
         <v>9</v>
       </c>
       <c r="B28" s="10"/>
       <c r="C28" s="1"/>
       <c r="D28" s="1"/>
       <c r="E28" s="3"/>
-      <c r="F28" s="29"/>
+      <c r="F28" s="27"/>
       <c r="G28" s="1"/>
     </row>
     <row r="29" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A29" s="27">
+      <c r="A29" s="25">
         <v>10</v>
       </c>
-      <c r="B29" s="32"/>
-      <c r="C29" s="27"/>
-      <c r="D29" s="27"/>
-      <c r="E29" s="20"/>
-      <c r="F29" s="32"/>
+      <c r="B29" s="30"/>
+      <c r="C29" s="25"/>
+      <c r="D29" s="25"/>
+      <c r="E29" s="18"/>
+      <c r="F29" s="30"/>
       <c r="G29" s="1"/>
     </row>
     <row r="30" spans="1:7" x14ac:dyDescent="0.25">
@@ -1054,7 +1261,7 @@
       <c r="C30" s="1"/>
       <c r="D30" s="1"/>
       <c r="E30" s="3"/>
-      <c r="F30" s="29"/>
+      <c r="F30" s="27"/>
       <c r="G30" s="1"/>
     </row>
     <row r="31" spans="1:7" x14ac:dyDescent="0.25">
@@ -1065,30 +1272,28 @@
       <c r="C31" s="1"/>
       <c r="D31" s="1"/>
       <c r="E31" s="3"/>
-      <c r="F31" s="29"/>
+      <c r="F31" s="27"/>
       <c r="G31" s="1"/>
     </row>
     <row r="32" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A32" s="1"/>
-      <c r="B32" s="10"/>
+      <c r="B32" s="32"/>
       <c r="C32" s="1"/>
+      <c r="D32" s="1"/>
       <c r="E32" s="3"/>
-      <c r="F32" s="14"/>
+      <c r="F32" s="32"/>
+      <c r="G32" s="1"/>
     </row>
     <row r="33" spans="1:7" ht="20.25" x14ac:dyDescent="0.3">
-      <c r="A33" s="6"/>
-      <c r="B33" s="18" t="s">
+      <c r="B33" s="17" t="s">
         <v>15</v>
       </c>
-      <c r="C33" s="3"/>
-      <c r="D33" s="3"/>
-      <c r="E33" s="3"/>
-    </row>
-    <row r="34" spans="1:7" s="8" customFormat="1" ht="15" x14ac:dyDescent="0.25">
+    </row>
+    <row r="34" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A34" s="7" t="s">
         <v>1</v>
       </c>
-      <c r="B34" s="15" t="s">
+      <c r="B34" s="14" t="s">
         <v>16</v>
       </c>
       <c r="C34" s="7" t="s">
@@ -1101,364 +1306,657 @@
         <v>10</v>
       </c>
       <c r="F34" s="7" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="G34" s="7" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="35" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A35" s="3">
-        <v>1</v>
-      </c>
-      <c r="B35" s="16"/>
-      <c r="C35" s="13"/>
-      <c r="D35" s="5"/>
-      <c r="E35" s="13"/>
-      <c r="F35" s="10"/>
-    </row>
-    <row r="36" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A36" s="3">
+    <row r="35" spans="1:7" ht="31.5" x14ac:dyDescent="0.25">
+      <c r="A35" s="1">
+        <v>1</v>
+      </c>
+      <c r="B35" s="32" t="s">
+        <v>69</v>
+      </c>
+      <c r="C35" s="1" t="s">
+        <v>72</v>
+      </c>
+      <c r="D35" t="s">
+        <v>73</v>
+      </c>
+      <c r="E35" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="F35" s="13"/>
+    </row>
+    <row r="36" spans="1:7" ht="31.5" x14ac:dyDescent="0.25">
+      <c r="A36" s="1">
         <v>2</v>
       </c>
-      <c r="B36" s="16"/>
-      <c r="C36" s="13"/>
-      <c r="D36" s="5"/>
-      <c r="E36" s="13"/>
-      <c r="F36" s="10"/>
-    </row>
-    <row r="37" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A37" s="3">
+      <c r="B36" s="32" t="s">
+        <v>70</v>
+      </c>
+      <c r="C36" s="1" t="s">
+        <v>72</v>
+      </c>
+      <c r="D36" t="s">
+        <v>73</v>
+      </c>
+      <c r="E36" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="F36" s="13"/>
+    </row>
+    <row r="37" spans="1:7" ht="31.5" x14ac:dyDescent="0.25">
+      <c r="A37" s="1">
         <v>3</v>
       </c>
-      <c r="B37" s="5"/>
-      <c r="C37" s="3"/>
-      <c r="D37" s="3"/>
-      <c r="E37" s="3"/>
-      <c r="F37" s="10"/>
+      <c r="B37" s="32" t="s">
+        <v>71</v>
+      </c>
+      <c r="C37" s="1" t="s">
+        <v>72</v>
+      </c>
+      <c r="D37" t="s">
+        <v>73</v>
+      </c>
+      <c r="E37" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="F37" s="13"/>
     </row>
     <row r="38" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A38" s="3">
+      <c r="A38" s="1">
         <v>4</v>
       </c>
-      <c r="B38" s="5"/>
-      <c r="C38" s="3"/>
-      <c r="D38" s="3"/>
-      <c r="E38" s="3"/>
-      <c r="F38" s="10"/>
-    </row>
-    <row r="40" spans="1:7" ht="20.25" x14ac:dyDescent="0.3">
-      <c r="B40" s="6" t="s">
+      <c r="B38" s="31" t="s">
+        <v>74</v>
+      </c>
+      <c r="C38" s="1" t="s">
+        <v>72</v>
+      </c>
+      <c r="D38" t="s">
+        <v>73</v>
+      </c>
+      <c r="E38" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="F38" s="13"/>
+    </row>
+    <row r="39" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A39" s="1">
+        <v>5</v>
+      </c>
+      <c r="B39" s="31"/>
+      <c r="C39" s="1"/>
+      <c r="E39" s="1"/>
+      <c r="F39" s="13"/>
+    </row>
+    <row r="40" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A40" s="1">
+        <v>6</v>
+      </c>
+      <c r="B40" s="32"/>
+      <c r="C40" s="1"/>
+      <c r="E40" s="1"/>
+      <c r="F40" s="13"/>
+    </row>
+    <row r="41" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A41" s="1">
+        <v>7</v>
+      </c>
+      <c r="B41" s="32"/>
+      <c r="C41" s="1"/>
+      <c r="E41" s="1"/>
+      <c r="F41" s="13"/>
+    </row>
+    <row r="42" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B42" s="37"/>
+      <c r="C42" s="38"/>
+      <c r="F42" s="13"/>
+      <c r="G42" s="13"/>
+    </row>
+    <row r="43" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A43" s="1"/>
+      <c r="B43" s="10"/>
+      <c r="C43" s="1"/>
+      <c r="E43" s="3"/>
+      <c r="F43" s="13"/>
+    </row>
+    <row r="44" spans="1:7" ht="20.25" x14ac:dyDescent="0.3">
+      <c r="A44" s="6"/>
+      <c r="B44" s="17" t="s">
         <v>14</v>
       </c>
-    </row>
-    <row r="41" spans="1:7" s="8" customFormat="1" ht="15" x14ac:dyDescent="0.25">
-      <c r="A41" s="7" t="s">
-        <v>1</v>
-      </c>
-      <c r="B41" s="15" t="s">
+      <c r="C44" s="3"/>
+      <c r="D44" s="3"/>
+      <c r="E44" s="3"/>
+    </row>
+    <row r="45" spans="1:7" s="8" customFormat="1" ht="15" x14ac:dyDescent="0.25">
+      <c r="A45" s="7" t="s">
+        <v>1</v>
+      </c>
+      <c r="B45" s="14" t="s">
         <v>16</v>
       </c>
-      <c r="C41" s="7" t="s">
+      <c r="C45" s="7" t="s">
         <v>22</v>
       </c>
-      <c r="D41" s="7" t="s">
+      <c r="D45" s="7" t="s">
         <v>9</v>
       </c>
-      <c r="E41" s="7" t="s">
+      <c r="E45" s="7" t="s">
         <v>10</v>
       </c>
-      <c r="F41" s="7" t="s">
+      <c r="F45" s="7" t="s">
         <v>12</v>
       </c>
-      <c r="G41" s="7" t="s">
+      <c r="G45" s="7" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="42" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A42" s="9">
-        <v>1</v>
-      </c>
-      <c r="B42" s="11"/>
-      <c r="C42" s="9"/>
-      <c r="D42" s="11"/>
-      <c r="E42" s="9"/>
-      <c r="F42" s="9"/>
-      <c r="G42" s="11"/>
-    </row>
-    <row r="43" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A43" s="9">
+    <row r="46" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A46" s="3">
+        <v>1</v>
+      </c>
+      <c r="B46" s="42" t="s">
+        <v>49</v>
+      </c>
+      <c r="C46" s="15">
+        <v>6</v>
+      </c>
+      <c r="D46" s="5" t="s">
+        <v>53</v>
+      </c>
+      <c r="E46" s="12" t="s">
+        <v>67</v>
+      </c>
+      <c r="F46" s="10"/>
+    </row>
+    <row r="47" spans="1:7" ht="29.25" x14ac:dyDescent="0.25">
+      <c r="A47" s="3">
         <v>2</v>
       </c>
-      <c r="B43" s="11"/>
-      <c r="C43" s="9"/>
-      <c r="D43" s="11"/>
-      <c r="E43" s="9"/>
-      <c r="F43" s="9"/>
-      <c r="G43" s="10"/>
-    </row>
-    <row r="44" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A44" s="9">
+      <c r="B47" s="40" t="s">
+        <v>50</v>
+      </c>
+      <c r="C47" s="15">
+        <v>6</v>
+      </c>
+      <c r="D47" s="5" t="s">
+        <v>53</v>
+      </c>
+      <c r="E47" s="12" t="s">
+        <v>67</v>
+      </c>
+      <c r="F47" s="10"/>
+    </row>
+    <row r="48" spans="1:7" ht="28.5" x14ac:dyDescent="0.25">
+      <c r="A48" s="3">
         <v>3</v>
       </c>
-      <c r="B44" s="11"/>
-      <c r="C44" s="9"/>
-      <c r="D44" s="11"/>
-      <c r="E44" s="9"/>
-      <c r="F44" s="9"/>
-      <c r="G44" s="10"/>
-    </row>
-    <row r="45" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A45" s="9">
+      <c r="B48" s="42" t="s">
+        <v>51</v>
+      </c>
+      <c r="C48" s="15">
+        <v>6</v>
+      </c>
+      <c r="D48" s="5" t="s">
+        <v>53</v>
+      </c>
+      <c r="E48" s="12" t="s">
+        <v>67</v>
+      </c>
+      <c r="F48" s="10"/>
+    </row>
+    <row r="49" spans="1:7" ht="31.5" x14ac:dyDescent="0.25">
+      <c r="A49" s="3">
         <v>4</v>
       </c>
-      <c r="B45" s="11"/>
-      <c r="C45" s="19"/>
-      <c r="D45" s="11"/>
-      <c r="E45" s="9"/>
-      <c r="F45" s="11"/>
-      <c r="G45" s="10"/>
-    </row>
-    <row r="46" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A46" s="9">
+      <c r="B49" s="43" t="s">
+        <v>52</v>
+      </c>
+      <c r="C49" s="15">
+        <v>6</v>
+      </c>
+      <c r="D49" s="5" t="s">
+        <v>53</v>
+      </c>
+      <c r="E49" s="12" t="s">
+        <v>67</v>
+      </c>
+      <c r="F49" s="10"/>
+    </row>
+    <row r="50" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A50" s="3">
         <v>5</v>
       </c>
-      <c r="B46" s="11"/>
-      <c r="C46" s="9"/>
-      <c r="D46" s="11"/>
-      <c r="E46" s="9"/>
-      <c r="F46" s="11"/>
-      <c r="G46" s="10"/>
-    </row>
-    <row r="48" spans="1:7" ht="20.25" x14ac:dyDescent="0.3">
-      <c r="B48" s="6" t="s">
+      <c r="B50" s="43" t="s">
+        <v>54</v>
+      </c>
+      <c r="C50" s="5">
+        <v>1</v>
+      </c>
+      <c r="D50" s="3" t="s">
+        <v>60</v>
+      </c>
+      <c r="E50" s="12" t="s">
+        <v>67</v>
+      </c>
+      <c r="F50" s="32"/>
+    </row>
+    <row r="51" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A51" s="3">
+        <v>6</v>
+      </c>
+      <c r="B51" s="39" t="s">
+        <v>55</v>
+      </c>
+      <c r="C51" s="5">
+        <v>1</v>
+      </c>
+      <c r="D51" s="3" t="s">
+        <v>60</v>
+      </c>
+      <c r="E51" s="12" t="s">
+        <v>67</v>
+      </c>
+      <c r="F51" s="32"/>
+    </row>
+    <row r="52" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A52" s="3">
+        <v>7</v>
+      </c>
+      <c r="B52" s="39" t="s">
+        <v>56</v>
+      </c>
+      <c r="C52" s="5">
+        <v>1</v>
+      </c>
+      <c r="D52" s="3" t="s">
+        <v>60</v>
+      </c>
+      <c r="E52" s="12" t="s">
+        <v>67</v>
+      </c>
+      <c r="F52" s="32"/>
+    </row>
+    <row r="53" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A53" s="3">
+        <v>8</v>
+      </c>
+      <c r="B53" s="41" t="s">
+        <v>57</v>
+      </c>
+      <c r="C53" s="5">
+        <v>1</v>
+      </c>
+      <c r="D53" s="3" t="s">
+        <v>60</v>
+      </c>
+      <c r="E53" s="12" t="s">
+        <v>67</v>
+      </c>
+      <c r="F53" s="32"/>
+    </row>
+    <row r="54" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A54" s="3">
+        <v>9</v>
+      </c>
+      <c r="B54" s="39" t="s">
+        <v>58</v>
+      </c>
+      <c r="C54" s="5">
+        <v>1</v>
+      </c>
+      <c r="D54" s="3" t="s">
+        <v>60</v>
+      </c>
+      <c r="E54" s="12" t="s">
+        <v>67</v>
+      </c>
+      <c r="F54" s="32"/>
+    </row>
+    <row r="55" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A55" s="3">
+        <v>10</v>
+      </c>
+      <c r="B55" s="39" t="s">
+        <v>59</v>
+      </c>
+      <c r="C55" s="5">
+        <v>1</v>
+      </c>
+      <c r="D55" s="3" t="s">
+        <v>60</v>
+      </c>
+      <c r="E55" s="12" t="s">
+        <v>67</v>
+      </c>
+      <c r="F55" s="32"/>
+    </row>
+    <row r="56" spans="1:7" ht="31.5" x14ac:dyDescent="0.25">
+      <c r="A56" s="3">
+        <v>11</v>
+      </c>
+      <c r="B56" s="13" t="s">
+        <v>62</v>
+      </c>
+      <c r="C56" s="32">
+        <v>4</v>
+      </c>
+      <c r="D56" s="3" t="s">
+        <v>63</v>
+      </c>
+      <c r="E56" s="12" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="57" spans="1:7" ht="47.25" x14ac:dyDescent="0.25">
+      <c r="A57" s="3">
+        <v>12</v>
+      </c>
+      <c r="B57" s="13" t="s">
+        <v>61</v>
+      </c>
+      <c r="C57" s="11">
+        <v>4</v>
+      </c>
+      <c r="D57" s="3" t="s">
+        <v>63</v>
+      </c>
+      <c r="E57" s="12" t="s">
+        <v>67</v>
+      </c>
+      <c r="F57" s="9"/>
+      <c r="G57" s="10"/>
+    </row>
+    <row r="58" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A58" s="3">
+        <v>13</v>
+      </c>
+      <c r="B58" s="39" t="s">
+        <v>64</v>
+      </c>
+      <c r="C58" s="11">
+        <v>2</v>
+      </c>
+      <c r="D58" s="11" t="s">
+        <v>66</v>
+      </c>
+      <c r="E58" s="12" t="s">
+        <v>67</v>
+      </c>
+      <c r="F58" s="9"/>
+      <c r="G58" s="10"/>
+    </row>
+    <row r="59" spans="1:7" ht="29.25" x14ac:dyDescent="0.25">
+      <c r="A59" s="3">
+        <v>14</v>
+      </c>
+      <c r="B59" s="40" t="s">
+        <v>65</v>
+      </c>
+      <c r="C59" s="45">
+        <v>2</v>
+      </c>
+      <c r="D59" s="11" t="s">
+        <v>66</v>
+      </c>
+      <c r="E59" s="12" t="s">
+        <v>67</v>
+      </c>
+      <c r="F59" s="11"/>
+      <c r="G59" s="10"/>
+    </row>
+    <row r="60" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A60" s="3">
+        <v>15</v>
+      </c>
+      <c r="B60" s="44"/>
+      <c r="C60" s="11"/>
+      <c r="D60" s="11"/>
+      <c r="E60" s="9"/>
+      <c r="F60" s="11"/>
+      <c r="G60" s="10"/>
+    </row>
+    <row r="61" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A61" s="3">
+        <v>16</v>
+      </c>
+      <c r="C61" s="13"/>
+    </row>
+    <row r="62" spans="1:7" ht="20.25" x14ac:dyDescent="0.3">
+      <c r="B62" s="6" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="49" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A49" s="7" t="s">
-        <v>1</v>
-      </c>
-      <c r="B49" s="15" t="s">
+    <row r="63" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A63" s="7" t="s">
+        <v>1</v>
+      </c>
+      <c r="B63" s="14" t="s">
         <v>16</v>
       </c>
-      <c r="C49" s="7" t="s">
+      <c r="C63" s="7" t="s">
         <v>22</v>
       </c>
-      <c r="D49" s="7" t="s">
+      <c r="D63" s="7" t="s">
         <v>9</v>
       </c>
-      <c r="E49" s="7" t="s">
+      <c r="E63" s="7" t="s">
         <v>10</v>
       </c>
-      <c r="F49" s="7" t="s">
+      <c r="F63" s="7" t="s">
         <v>13</v>
       </c>
-      <c r="G49" s="7" t="s">
+      <c r="G63" s="7" t="s">
         <v>23</v>
       </c>
-    </row>
-    <row r="50" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A50" s="1">
-        <v>1</v>
-      </c>
-      <c r="B50" s="10"/>
-      <c r="C50" s="1"/>
-      <c r="E50" s="1"/>
-      <c r="F50" s="14"/>
-    </row>
-    <row r="51" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A51" s="1">
-        <v>2</v>
-      </c>
-      <c r="B51" s="10"/>
-      <c r="C51" s="1"/>
-      <c r="E51" s="1"/>
-      <c r="F51" s="14"/>
-    </row>
-    <row r="52" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A52" s="1">
-        <v>3</v>
-      </c>
-      <c r="B52" s="10"/>
-      <c r="C52" s="1"/>
-      <c r="E52" s="1"/>
-      <c r="F52" s="14"/>
-    </row>
-    <row r="53" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A53" s="1">
-        <v>4</v>
-      </c>
-      <c r="B53" s="28"/>
-      <c r="C53" s="1"/>
-      <c r="E53" s="1"/>
-      <c r="F53" s="14"/>
-    </row>
-    <row r="54" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A54" s="1">
-        <v>5</v>
-      </c>
-      <c r="B54" s="28"/>
-      <c r="C54" s="1"/>
-      <c r="E54" s="1"/>
-      <c r="F54" s="14"/>
-    </row>
-    <row r="55" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A55" s="1">
-        <v>6</v>
-      </c>
-      <c r="B55" s="10"/>
-      <c r="C55" s="1"/>
-      <c r="E55" s="1"/>
-      <c r="F55" s="14"/>
-    </row>
-    <row r="56" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A56" s="1">
-        <v>7</v>
-      </c>
-      <c r="B56" s="10"/>
-      <c r="C56" s="1"/>
-      <c r="E56" s="1"/>
-      <c r="F56" s="14"/>
-    </row>
-    <row r="57" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="B57" s="37"/>
-      <c r="C57" s="38"/>
-      <c r="F57" s="14"/>
-      <c r="G57" s="14"/>
-    </row>
-    <row r="59" spans="1:7" ht="20.25" x14ac:dyDescent="0.3">
-      <c r="B59" s="18" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="60" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A60" s="7" t="s">
-        <v>1</v>
-      </c>
-      <c r="B60" s="15" t="s">
-        <v>16</v>
-      </c>
-      <c r="C60" s="7" t="s">
-        <v>22</v>
-      </c>
-      <c r="D60" s="7" t="s">
-        <v>9</v>
-      </c>
-      <c r="E60" s="7" t="s">
-        <v>10</v>
-      </c>
-      <c r="F60" s="7" t="s">
-        <v>13</v>
-      </c>
-      <c r="G60" s="7" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="61" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A61" s="1">
-        <v>1</v>
-      </c>
-      <c r="C61" s="1"/>
-    </row>
-    <row r="62" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A62" s="1">
-        <v>2</v>
-      </c>
-      <c r="C62" s="1"/>
-    </row>
-    <row r="63" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A63" s="1">
-        <v>3</v>
-      </c>
-      <c r="C63" s="1"/>
     </row>
     <row r="64" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A64" s="1">
-        <v>4</v>
-      </c>
+        <v>1</v>
+      </c>
+      <c r="B64" s="10"/>
       <c r="C64" s="1"/>
+      <c r="E64" s="1"/>
+      <c r="F64" s="13"/>
     </row>
     <row r="65" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A65" s="1">
+        <v>2</v>
+      </c>
+      <c r="B65" s="10"/>
+      <c r="C65" s="1"/>
+      <c r="E65" s="1"/>
+      <c r="F65" s="13"/>
+    </row>
+    <row r="66" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A66" s="1">
+        <v>3</v>
+      </c>
+      <c r="B66" s="10"/>
+      <c r="C66" s="1"/>
+      <c r="E66" s="1"/>
+      <c r="F66" s="13"/>
+    </row>
+    <row r="67" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A67" s="1">
+        <v>4</v>
+      </c>
+      <c r="B67" s="26"/>
+      <c r="C67" s="1"/>
+      <c r="E67" s="1"/>
+      <c r="F67" s="13"/>
+    </row>
+    <row r="68" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A68" s="1">
         <v>5</v>
       </c>
-      <c r="C65" s="1"/>
-    </row>
-    <row r="66" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="C66" s="1"/>
-    </row>
-    <row r="67" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="C67" s="1"/>
-    </row>
-    <row r="68" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B68" s="26"/>
       <c r="C68" s="1"/>
-    </row>
-    <row r="69" spans="1:7" ht="20.25" x14ac:dyDescent="0.3">
-      <c r="B69" s="18" t="s">
-        <v>39</v>
-      </c>
+      <c r="E68" s="1"/>
+      <c r="F68" s="13"/>
+    </row>
+    <row r="69" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A69" s="1">
+        <v>6</v>
+      </c>
+      <c r="B69" s="10"/>
+      <c r="C69" s="1"/>
+      <c r="E69" s="1"/>
+      <c r="F69" s="13"/>
     </row>
     <row r="70" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A70" s="7" t="s">
-        <v>1</v>
-      </c>
-      <c r="B70" s="15" t="s">
+      <c r="A70" s="1">
+        <v>7</v>
+      </c>
+      <c r="B70" s="10"/>
+      <c r="C70" s="1"/>
+      <c r="E70" s="1"/>
+      <c r="F70" s="13"/>
+    </row>
+    <row r="71" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B71" s="37"/>
+      <c r="C71" s="38"/>
+      <c r="F71" s="13"/>
+      <c r="G71" s="13"/>
+    </row>
+    <row r="73" spans="1:7" ht="20.25" x14ac:dyDescent="0.3">
+      <c r="B73" s="17" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="74" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A74" s="7" t="s">
+        <v>1</v>
+      </c>
+      <c r="B74" s="14" t="s">
         <v>16</v>
       </c>
-      <c r="C70" s="7" t="s">
+      <c r="C74" s="7" t="s">
         <v>22</v>
       </c>
-      <c r="D70" s="7" t="s">
+      <c r="D74" s="7" t="s">
         <v>9</v>
       </c>
-      <c r="E70" s="7" t="s">
+      <c r="E74" s="7" t="s">
         <v>10</v>
       </c>
-      <c r="F70" s="7" t="s">
+      <c r="F74" s="7" t="s">
         <v>13</v>
       </c>
-      <c r="G70" s="7" t="s">
+      <c r="G74" s="7" t="s">
         <v>23</v>
       </c>
-    </row>
-    <row r="71" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A71" s="1">
-        <v>1</v>
-      </c>
-      <c r="C71" s="1"/>
-    </row>
-    <row r="72" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A72" s="1">
-        <v>2</v>
-      </c>
-      <c r="C72" s="1"/>
-    </row>
-    <row r="73" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A73" s="1">
-        <v>3</v>
-      </c>
-      <c r="C73" s="1"/>
-    </row>
-    <row r="74" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A74" s="1">
-        <v>4</v>
-      </c>
-      <c r="C74" s="1"/>
     </row>
     <row r="75" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A75" s="1">
+        <v>1</v>
+      </c>
+      <c r="C75" s="1"/>
+    </row>
+    <row r="76" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A76" s="1">
+        <v>2</v>
+      </c>
+      <c r="C76" s="1"/>
+    </row>
+    <row r="77" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A77" s="1">
+        <v>3</v>
+      </c>
+      <c r="C77" s="1"/>
+    </row>
+    <row r="78" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A78" s="1">
+        <v>4</v>
+      </c>
+      <c r="C78" s="1"/>
+    </row>
+    <row r="79" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A79" s="1">
         <v>5</v>
       </c>
-      <c r="C75" s="1"/>
+      <c r="C79" s="1"/>
+    </row>
+    <row r="80" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="C80" s="1"/>
+    </row>
+    <row r="81" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="C81" s="1"/>
+    </row>
+    <row r="82" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="C82" s="1"/>
+    </row>
+    <row r="83" spans="1:7" ht="20.25" x14ac:dyDescent="0.3">
+      <c r="B83" s="17" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="84" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A84" s="7" t="s">
+        <v>1</v>
+      </c>
+      <c r="B84" s="14" t="s">
+        <v>16</v>
+      </c>
+      <c r="C84" s="7" t="s">
+        <v>22</v>
+      </c>
+      <c r="D84" s="7" t="s">
+        <v>9</v>
+      </c>
+      <c r="E84" s="7" t="s">
+        <v>10</v>
+      </c>
+      <c r="F84" s="7" t="s">
+        <v>13</v>
+      </c>
+      <c r="G84" s="7" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="85" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A85" s="1">
+        <v>1</v>
+      </c>
+      <c r="C85" s="1"/>
+    </row>
+    <row r="86" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A86" s="1">
+        <v>2</v>
+      </c>
+      <c r="C86" s="1"/>
+    </row>
+    <row r="87" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A87" s="1">
+        <v>3</v>
+      </c>
+      <c r="C87" s="1"/>
+    </row>
+    <row r="88" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A88" s="1">
+        <v>4</v>
+      </c>
+      <c r="C88" s="1"/>
+    </row>
+    <row r="89" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A89" s="1">
+        <v>5</v>
+      </c>
+      <c r="C89" s="1"/>
     </row>
   </sheetData>
-  <mergeCells count="5">
+  <mergeCells count="6">
     <mergeCell ref="C1:E1"/>
     <mergeCell ref="C2:E2"/>
     <mergeCell ref="C7:E7"/>
     <mergeCell ref="B3:B7"/>
-    <mergeCell ref="B57:C57"/>
+    <mergeCell ref="B71:C71"/>
+    <mergeCell ref="B42:C42"/>
   </mergeCells>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
sp3 burn chart edits; method for sending ics email created
</commit_message>
<xml_diff>
--- a/Documentation/backlogs/masterProductBacklog.xlsx
+++ b/Documentation/backlogs/masterProductBacklog.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="222" uniqueCount="120">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="239" uniqueCount="125">
   <si>
     <t>Sprints</t>
   </si>
@@ -331,9 +331,6 @@
     <t>Create a login/user table(s)</t>
   </si>
   <si>
-    <t xml:space="preserve">     hashing/security for passowords</t>
-  </si>
-  <si>
     <t>Naif, Tom</t>
   </si>
   <si>
@@ -373,13 +370,31 @@
     <t>4,6</t>
   </si>
   <si>
-    <t>done</t>
-  </si>
-  <si>
     <t>waiting</t>
   </si>
   <si>
     <t>In Progress (75%)</t>
+  </si>
+  <si>
+    <t>waiting for data</t>
+  </si>
+  <si>
+    <t>In Progress (90%)</t>
+  </si>
+  <si>
+    <t>In Progress (70%)</t>
+  </si>
+  <si>
+    <t>In Progress (85%)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">     hashing/security for passwords</t>
+  </si>
+  <si>
+    <t>Tom, Andrew</t>
+  </si>
+  <si>
+    <t>Create different messages for student professor in ics email</t>
   </si>
 </sst>
 </file>
@@ -494,7 +509,7 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="53">
+  <cellXfs count="56">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -615,23 +630,30 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
   </cellXfs>
   <cellStyles count="6">
     <cellStyle name="Followed Hyperlink" xfId="3" builtinId="9" hidden="1"/>
@@ -976,10 +998,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G100"/>
+  <dimension ref="A1:G101"/>
   <sheetViews>
-    <sheetView tabSelected="1" showRuler="0" zoomScale="78" zoomScaleNormal="78" workbookViewId="0">
-      <selection activeCell="E31" sqref="E31"/>
+    <sheetView tabSelected="1" showRuler="0" topLeftCell="A58" zoomScale="78" zoomScaleNormal="78" workbookViewId="0">
+      <selection activeCell="B79" sqref="B79"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.125" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -999,11 +1021,11 @@
       <c r="B1" s="21" t="s">
         <v>32</v>
       </c>
-      <c r="C1" s="48" t="s">
+      <c r="C1" s="49" t="s">
         <v>37</v>
       </c>
-      <c r="D1" s="48"/>
-      <c r="E1" s="48"/>
+      <c r="D1" s="49"/>
+      <c r="E1" s="49"/>
       <c r="F1" s="20" t="s">
         <v>34</v>
       </c>
@@ -1013,14 +1035,14 @@
       <c r="B2" s="20" t="s">
         <v>33</v>
       </c>
-      <c r="C2" s="49"/>
-      <c r="D2" s="49"/>
-      <c r="E2" s="49"/>
+      <c r="C2" s="50"/>
+      <c r="D2" s="50"/>
+      <c r="E2" s="50"/>
       <c r="F2" s="20"/>
     </row>
     <row r="3" spans="1:7" ht="18" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A3" s="20"/>
-      <c r="B3" s="50"/>
+      <c r="B3" s="51"/>
       <c r="C3" s="23" t="s">
         <v>24</v>
       </c>
@@ -1032,7 +1054,7 @@
     </row>
     <row r="4" spans="1:7" ht="18" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A4" s="20"/>
-      <c r="B4" s="50"/>
+      <c r="B4" s="51"/>
       <c r="C4" s="22" t="s">
         <v>27</v>
       </c>
@@ -1044,7 +1066,7 @@
     </row>
     <row r="5" spans="1:7" ht="18" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A5" s="20"/>
-      <c r="B5" s="50"/>
+      <c r="B5" s="51"/>
       <c r="C5" s="22" t="s">
         <v>28</v>
       </c>
@@ -1056,7 +1078,7 @@
     </row>
     <row r="6" spans="1:7" ht="18" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A6" s="20"/>
-      <c r="B6" s="50"/>
+      <c r="B6" s="51"/>
       <c r="C6" s="22" t="s">
         <v>23</v>
       </c>
@@ -1068,7 +1090,7 @@
     </row>
     <row r="7" spans="1:7" ht="18" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A7" s="2"/>
-      <c r="B7" s="50"/>
+      <c r="B7" s="51"/>
       <c r="C7" s="40" t="s">
         <v>78</v>
       </c>
@@ -1118,8 +1140,8 @@
       <c r="E10" s="3" t="s">
         <v>66</v>
       </c>
-      <c r="F10" s="46"/>
-      <c r="G10" s="46"/>
+      <c r="F10" s="54"/>
+      <c r="G10" s="54"/>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A11" s="1">
@@ -1137,10 +1159,10 @@
       <c r="E11" s="3" t="s">
         <v>65</v>
       </c>
-      <c r="F11" s="47" t="s">
+      <c r="F11" s="55" t="s">
         <v>73</v>
       </c>
-      <c r="G11" s="47"/>
+      <c r="G11" s="55"/>
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A12" s="1">
@@ -1156,8 +1178,8 @@
         <v>42486</v>
       </c>
       <c r="E12" s="12"/>
-      <c r="F12" s="46"/>
-      <c r="G12" s="46"/>
+      <c r="F12" s="54"/>
+      <c r="G12" s="54"/>
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A13" s="1">
@@ -1173,8 +1195,8 @@
         <v>42493</v>
       </c>
       <c r="E13" s="12"/>
-      <c r="F13" s="46"/>
-      <c r="G13" s="46"/>
+      <c r="F13" s="54"/>
+      <c r="G13" s="54"/>
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A14" s="1"/>
@@ -1182,8 +1204,8 @@
       <c r="C14" s="16"/>
       <c r="D14" s="16"/>
       <c r="E14" s="12"/>
-      <c r="F14" s="46"/>
-      <c r="G14" s="46"/>
+      <c r="F14" s="54"/>
+      <c r="G14" s="54"/>
     </row>
     <row r="15" spans="1:7" ht="15.6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A15" s="2"/>
@@ -1243,7 +1265,7 @@
       </c>
       <c r="D18" s="1"/>
       <c r="E18" s="1" t="s">
-        <v>119</v>
+        <v>117</v>
       </c>
       <c r="F18" s="1" t="s">
         <v>65</v>
@@ -1262,10 +1284,10 @@
       </c>
       <c r="D19" s="1"/>
       <c r="E19" s="1" t="s">
+        <v>117</v>
+      </c>
+      <c r="F19" s="1" t="s">
         <v>119</v>
-      </c>
-      <c r="F19" s="1" t="s">
-        <v>65</v>
       </c>
       <c r="G19" s="1"/>
     </row>
@@ -1284,7 +1306,7 @@
         <v>65</v>
       </c>
       <c r="F20" s="1" t="s">
-        <v>65</v>
+        <v>120</v>
       </c>
       <c r="G20" s="1"/>
     </row>
@@ -1303,7 +1325,7 @@
         <v>65</v>
       </c>
       <c r="F21" s="1" t="s">
-        <v>65</v>
+        <v>120</v>
       </c>
       <c r="G21" s="1"/>
     </row>
@@ -1322,7 +1344,7 @@
         <v>65</v>
       </c>
       <c r="F22" s="1" t="s">
-        <v>65</v>
+        <v>121</v>
       </c>
       <c r="G22" s="1"/>
     </row>
@@ -1338,7 +1360,7 @@
       </c>
       <c r="D23" s="25"/>
       <c r="E23" s="1" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
       <c r="F23" s="1" t="s">
         <v>65</v>
@@ -1357,7 +1379,7 @@
       </c>
       <c r="D24" s="1"/>
       <c r="E24" s="1" t="s">
-        <v>117</v>
+        <v>76</v>
       </c>
       <c r="F24" s="1" t="s">
         <v>76</v>
@@ -1575,8 +1597,8 @@
       <c r="F40" s="13"/>
     </row>
     <row r="41" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="B41" s="51"/>
-      <c r="C41" s="52"/>
+      <c r="B41" s="52"/>
+      <c r="C41" s="53"/>
       <c r="F41" s="13"/>
       <c r="G41" s="13"/>
     </row>
@@ -1657,7 +1679,7 @@
         <v>75</v>
       </c>
       <c r="G46" s="44" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
     </row>
     <row r="47" spans="1:7" ht="28.5" x14ac:dyDescent="0.25">
@@ -1794,7 +1816,7 @@
       </c>
       <c r="F53" s="31"/>
       <c r="G53" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
     </row>
     <row r="54" spans="1:7" x14ac:dyDescent="0.25">
@@ -1817,7 +1839,7 @@
         <v>81</v>
       </c>
       <c r="G54" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
     </row>
     <row r="55" spans="1:7" ht="31.5" x14ac:dyDescent="0.25">
@@ -1855,7 +1877,7 @@
       </c>
       <c r="F56" s="9"/>
       <c r="G56" s="44" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
     </row>
     <row r="57" spans="1:7" x14ac:dyDescent="0.25">
@@ -1866,7 +1888,7 @@
         <v>62</v>
       </c>
       <c r="C57" s="11" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="D57" s="11" t="s">
         <v>64</v>
@@ -1956,7 +1978,9 @@
       <c r="D63" s="1" t="s">
         <v>85</v>
       </c>
-      <c r="E63" s="1"/>
+      <c r="E63" s="1" t="s">
+        <v>65</v>
+      </c>
       <c r="F63" s="13"/>
     </row>
     <row r="64" spans="1:7" x14ac:dyDescent="0.25">
@@ -1967,13 +1991,15 @@
         <v>86</v>
       </c>
       <c r="C64" s="1" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="D64" s="1" t="s">
         <v>61</v>
       </c>
       <c r="E64" s="1"/>
-      <c r="F64" s="13"/>
+      <c r="F64" s="13" t="s">
+        <v>118</v>
+      </c>
     </row>
     <row r="65" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A65" s="1">
@@ -1983,13 +2009,15 @@
         <v>87</v>
       </c>
       <c r="C65" s="1" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="D65" s="1" t="s">
         <v>61</v>
       </c>
       <c r="E65" s="1"/>
-      <c r="F65" s="13"/>
+      <c r="F65" s="13" t="s">
+        <v>118</v>
+      </c>
     </row>
     <row r="66" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A66" s="1">
@@ -1999,12 +2027,14 @@
         <v>88</v>
       </c>
       <c r="C66" s="1" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="D66" s="1" t="s">
         <v>89</v>
       </c>
-      <c r="E66" s="1"/>
+      <c r="E66" s="1" t="s">
+        <v>76</v>
+      </c>
       <c r="F66" s="13"/>
     </row>
     <row r="67" spans="1:7" x14ac:dyDescent="0.25">
@@ -2015,12 +2045,14 @@
         <v>90</v>
       </c>
       <c r="C67" s="1" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="D67" s="1" t="s">
         <v>58</v>
       </c>
-      <c r="E67" s="1"/>
+      <c r="E67" s="48">
+        <v>0.5</v>
+      </c>
       <c r="F67" s="13"/>
     </row>
     <row r="68" spans="1:7" x14ac:dyDescent="0.25">
@@ -2031,12 +2063,14 @@
         <v>91</v>
       </c>
       <c r="C68" s="1" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="D68" s="1" t="s">
         <v>92</v>
       </c>
-      <c r="E68" s="1"/>
+      <c r="E68" s="1" t="s">
+        <v>65</v>
+      </c>
       <c r="F68" s="13"/>
     </row>
     <row r="69" spans="1:7" x14ac:dyDescent="0.25">
@@ -2050,7 +2084,9 @@
       <c r="D69" s="1" t="s">
         <v>94</v>
       </c>
-      <c r="E69" s="1"/>
+      <c r="E69" s="1" t="s">
+        <v>65</v>
+      </c>
       <c r="F69" s="13"/>
     </row>
     <row r="70" spans="1:7" s="43" customFormat="1" x14ac:dyDescent="0.25">
@@ -2061,13 +2097,15 @@
         <v>95</v>
       </c>
       <c r="C70" s="1" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="D70" s="1" t="s">
         <v>96</v>
       </c>
       <c r="E70" s="1"/>
-      <c r="F70" s="13"/>
+      <c r="F70" s="13" t="s">
+        <v>118</v>
+      </c>
     </row>
     <row r="71" spans="1:7" s="43" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A71" s="1">
@@ -2081,7 +2119,9 @@
         <v>96</v>
       </c>
       <c r="E71" s="1"/>
-      <c r="F71" s="13"/>
+      <c r="F71" s="13" t="s">
+        <v>118</v>
+      </c>
     </row>
     <row r="72" spans="1:7" s="43" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A72" s="1">
@@ -2091,13 +2131,15 @@
         <v>98</v>
       </c>
       <c r="C72" s="1" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="D72" s="1" t="s">
         <v>99</v>
       </c>
       <c r="E72" s="1"/>
-      <c r="F72" s="13"/>
+      <c r="F72" s="13" t="s">
+        <v>118</v>
+      </c>
     </row>
     <row r="73" spans="1:7" s="43" customFormat="1" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A73" s="1">
@@ -2107,13 +2149,15 @@
         <v>100</v>
       </c>
       <c r="C73" s="1" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="D73" s="1" t="s">
         <v>99</v>
       </c>
       <c r="E73" s="1"/>
-      <c r="F73" s="13"/>
+      <c r="F73" s="13" t="s">
+        <v>118</v>
+      </c>
     </row>
     <row r="74" spans="1:7" s="43" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A74" s="1">
@@ -2124,9 +2168,11 @@
       </c>
       <c r="C74" s="1"/>
       <c r="D74" s="1" t="s">
-        <v>96</v>
-      </c>
-      <c r="E74" s="1"/>
+        <v>51</v>
+      </c>
+      <c r="E74" s="1" t="s">
+        <v>76</v>
+      </c>
       <c r="F74" s="13"/>
     </row>
     <row r="75" spans="1:7" s="43" customFormat="1" x14ac:dyDescent="0.25">
@@ -2140,9 +2186,11 @@
         <v>5</v>
       </c>
       <c r="D75" s="1" t="s">
-        <v>51</v>
-      </c>
-      <c r="E75" s="1"/>
+        <v>64</v>
+      </c>
+      <c r="E75" s="48">
+        <v>0.4</v>
+      </c>
       <c r="F75" s="13"/>
     </row>
     <row r="76" spans="1:7" s="43" customFormat="1" x14ac:dyDescent="0.25">
@@ -2150,15 +2198,17 @@
         <v>14</v>
       </c>
       <c r="B76" s="13" t="s">
-        <v>103</v>
+        <v>122</v>
       </c>
       <c r="C76" s="1">
         <v>5</v>
       </c>
       <c r="D76" s="1" t="s">
-        <v>104</v>
-      </c>
-      <c r="E76" s="1"/>
+        <v>103</v>
+      </c>
+      <c r="E76" s="48">
+        <v>0.4</v>
+      </c>
       <c r="F76" s="13"/>
     </row>
     <row r="77" spans="1:7" s="43" customFormat="1" x14ac:dyDescent="0.25">
@@ -2166,7 +2216,7 @@
         <v>15</v>
       </c>
       <c r="B77" s="13" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="C77" s="1">
         <v>5</v>
@@ -2174,7 +2224,9 @@
       <c r="D77" s="1" t="s">
         <v>89</v>
       </c>
-      <c r="E77" s="1"/>
+      <c r="E77" s="1" t="s">
+        <v>76</v>
+      </c>
       <c r="F77" s="13"/>
     </row>
     <row r="78" spans="1:7" s="43" customFormat="1" x14ac:dyDescent="0.25">
@@ -2182,20 +2234,22 @@
         <v>16</v>
       </c>
       <c r="B78" s="13" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="C78" s="1">
         <v>5</v>
       </c>
       <c r="D78" s="1" t="s">
-        <v>51</v>
-      </c>
-      <c r="E78" s="1"/>
+        <v>123</v>
+      </c>
+      <c r="E78" s="1" t="s">
+        <v>65</v>
+      </c>
       <c r="F78" s="13"/>
     </row>
     <row r="79" spans="1:7" s="44" customFormat="1" ht="29.25" x14ac:dyDescent="0.25">
       <c r="A79" s="3" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="B79" s="34" t="s">
         <v>63</v>
@@ -2214,7 +2268,7 @@
     </row>
     <row r="80" spans="1:7" s="44" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A80" s="3" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="B80" s="33" t="s">
         <v>56</v>
@@ -2225,17 +2279,17 @@
       <c r="D80" s="3" t="s">
         <v>58</v>
       </c>
-      <c r="E80" s="41">
-        <v>0.6</v>
+      <c r="E80" s="41" t="s">
+        <v>76</v>
       </c>
       <c r="F80" s="45"/>
       <c r="G80" s="44" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
     </row>
     <row r="81" spans="1:7" s="44" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A81" s="3" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="B81" s="33" t="s">
         <v>57</v>
@@ -2246,19 +2300,19 @@
       <c r="D81" s="3" t="s">
         <v>58</v>
       </c>
-      <c r="E81" s="41">
-        <v>0.6</v>
+      <c r="E81" s="41" t="s">
+        <v>76</v>
       </c>
       <c r="F81" s="45" t="s">
         <v>81</v>
       </c>
       <c r="G81" s="44" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
     </row>
     <row r="82" spans="1:7" s="44" customFormat="1" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A82" s="3" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="B82" s="34" t="s">
         <v>48</v>
@@ -2276,56 +2330,66 @@
         <v>75</v>
       </c>
     </row>
-    <row r="83" spans="1:7" s="44" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A83" s="3"/>
-      <c r="B83" s="33"/>
-      <c r="C83" s="5"/>
-      <c r="D83" s="3"/>
-      <c r="E83" s="41"/>
-      <c r="F83" s="45"/>
-    </row>
-    <row r="84" spans="1:7" ht="20.25" x14ac:dyDescent="0.3">
-      <c r="B84" s="17" t="s">
+    <row r="83" spans="1:7" s="47" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A83" s="3">
+        <v>19</v>
+      </c>
+      <c r="B83" s="34" t="s">
+        <v>124</v>
+      </c>
+      <c r="C83" s="15">
+        <v>1</v>
+      </c>
+      <c r="D83" s="5" t="s">
+        <v>58</v>
+      </c>
+      <c r="E83" s="41">
+        <v>0.1</v>
+      </c>
+      <c r="F83" s="46"/>
+    </row>
+    <row r="84" spans="1:7" s="44" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A84" s="3"/>
+      <c r="B84" s="33"/>
+      <c r="C84" s="5"/>
+      <c r="D84" s="3"/>
+      <c r="E84" s="41"/>
+      <c r="F84" s="45"/>
+    </row>
+    <row r="85" spans="1:7" ht="20.25" x14ac:dyDescent="0.3">
+      <c r="B85" s="17" t="s">
         <v>35</v>
       </c>
-      <c r="C84" s="43"/>
-      <c r="D84" s="43"/>
-      <c r="E84" s="43"/>
-    </row>
-    <row r="85" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A85" s="7" t="s">
+      <c r="C85" s="43"/>
+      <c r="D85" s="43"/>
+      <c r="E85" s="43"/>
+    </row>
+    <row r="86" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A86" s="7" t="s">
         <v>1</v>
       </c>
-      <c r="B85" s="14" t="s">
+      <c r="B86" s="14" t="s">
         <v>15</v>
       </c>
-      <c r="C85" s="7" t="s">
+      <c r="C86" s="7" t="s">
         <v>21</v>
       </c>
-      <c r="D85" s="7" t="s">
+      <c r="D86" s="7" t="s">
         <v>9</v>
       </c>
-      <c r="E85" s="7" t="s">
+      <c r="E86" s="7" t="s">
         <v>10</v>
       </c>
-      <c r="F85" s="7" t="s">
+      <c r="F86" s="7" t="s">
         <v>13</v>
       </c>
-      <c r="G85" s="7" t="s">
+      <c r="G86" s="7" t="s">
         <v>22</v>
       </c>
-    </row>
-    <row r="86" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A86" s="1">
-        <v>1</v>
-      </c>
-      <c r="C86" s="1"/>
-      <c r="D86" s="43"/>
-      <c r="E86" s="43"/>
     </row>
     <row r="87" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A87" s="1">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C87" s="1"/>
       <c r="D87" s="43"/>
@@ -2333,7 +2397,7 @@
     </row>
     <row r="88" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A88" s="1">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C88" s="1"/>
       <c r="D88" s="43"/>
@@ -2341,7 +2405,7 @@
     </row>
     <row r="89" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A89" s="1">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="C89" s="1"/>
       <c r="D89" s="43"/>
@@ -2349,14 +2413,19 @@
     </row>
     <row r="90" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A90" s="1">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C90" s="1"/>
       <c r="D90" s="43"/>
       <c r="E90" s="43"/>
     </row>
     <row r="91" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A91" s="1">
+        <v>5</v>
+      </c>
       <c r="C91" s="1"/>
+      <c r="D91" s="43"/>
+      <c r="E91" s="43"/>
     </row>
     <row r="92" spans="1:7" x14ac:dyDescent="0.25">
       <c r="C92" s="1"/>
@@ -2364,63 +2433,66 @@
     <row r="93" spans="1:7" x14ac:dyDescent="0.25">
       <c r="C93" s="1"/>
     </row>
-    <row r="94" spans="1:7" ht="20.25" x14ac:dyDescent="0.3">
-      <c r="B94" s="17" t="s">
+    <row r="94" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="C94" s="1"/>
+    </row>
+    <row r="95" spans="1:7" ht="20.25" x14ac:dyDescent="0.3">
+      <c r="B95" s="17" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="95" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A95" s="7" t="s">
+    <row r="96" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A96" s="7" t="s">
         <v>1</v>
       </c>
-      <c r="B95" s="14" t="s">
+      <c r="B96" s="14" t="s">
         <v>15</v>
       </c>
-      <c r="C95" s="7" t="s">
+      <c r="C96" s="7" t="s">
         <v>21</v>
       </c>
-      <c r="D95" s="7" t="s">
+      <c r="D96" s="7" t="s">
         <v>9</v>
       </c>
-      <c r="E95" s="7" t="s">
+      <c r="E96" s="7" t="s">
         <v>10</v>
       </c>
-      <c r="F95" s="7" t="s">
+      <c r="F96" s="7" t="s">
         <v>13</v>
       </c>
-      <c r="G95" s="7" t="s">
+      <c r="G96" s="7" t="s">
         <v>22</v>
       </c>
-    </row>
-    <row r="96" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A96" s="1">
-        <v>1</v>
-      </c>
-      <c r="C96" s="1"/>
     </row>
     <row r="97" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A97" s="1">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C97" s="1"/>
     </row>
     <row r="98" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A98" s="1">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C98" s="1"/>
     </row>
     <row r="99" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A99" s="1">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="C99" s="1"/>
     </row>
     <row r="100" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A100" s="1">
+        <v>4</v>
+      </c>
+      <c r="C100" s="1"/>
+    </row>
+    <row r="101" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A101" s="1">
         <v>5</v>
       </c>
-      <c r="C100" s="1"/>
+      <c r="C101" s="1"/>
     </row>
   </sheetData>
   <mergeCells count="9">

</xml_diff>

<commit_message>
completed two different emails functionality; created method to take and parse data to send ics email; refactored code.
</commit_message>
<xml_diff>
--- a/Documentation/backlogs/masterProductBacklog.xlsx
+++ b/Documentation/backlogs/masterProductBacklog.xlsx
@@ -1000,8 +1000,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G101"/>
   <sheetViews>
-    <sheetView tabSelected="1" showRuler="0" topLeftCell="A58" zoomScale="78" zoomScaleNormal="78" workbookViewId="0">
-      <selection activeCell="B79" sqref="B79"/>
+    <sheetView tabSelected="1" showRuler="0" topLeftCell="A60" zoomScale="78" zoomScaleNormal="78" workbookViewId="0">
+      <selection activeCell="F81" sqref="F81"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.125" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -2050,8 +2050,8 @@
       <c r="D67" s="1" t="s">
         <v>58</v>
       </c>
-      <c r="E67" s="48">
-        <v>0.5</v>
+      <c r="E67" s="48" t="s">
+        <v>76</v>
       </c>
       <c r="F67" s="13"/>
     </row>
@@ -2283,9 +2283,6 @@
         <v>76</v>
       </c>
       <c r="F80" s="45"/>
-      <c r="G80" s="44" t="s">
-        <v>106</v>
-      </c>
     </row>
     <row r="81" spans="1:7" s="44" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A81" s="3" t="s">
@@ -2306,9 +2303,6 @@
       <c r="F81" s="45" t="s">
         <v>81</v>
       </c>
-      <c r="G81" s="44" t="s">
-        <v>106</v>
-      </c>
     </row>
     <row r="82" spans="1:7" s="44" customFormat="1" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A82" s="3" t="s">
@@ -2343,8 +2337,8 @@
       <c r="D83" s="5" t="s">
         <v>58</v>
       </c>
-      <c r="E83" s="41">
-        <v>0.1</v>
+      <c r="E83" s="41" t="s">
+        <v>76</v>
       </c>
       <c r="F83" s="46"/>
     </row>

</xml_diff>

<commit_message>
updated backlog for end of sprint 3 and for the start of sprint 4.
</commit_message>
<xml_diff>
--- a/Documentation/backlogs/masterProductBacklog.xlsx
+++ b/Documentation/backlogs/masterProductBacklog.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="239" uniqueCount="125">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="294" uniqueCount="142">
   <si>
     <t>Sprints</t>
   </si>
@@ -376,9 +376,6 @@
     <t>In Progress (75%)</t>
   </si>
   <si>
-    <t>waiting for data</t>
-  </si>
-  <si>
     <t>In Progress (90%)</t>
   </si>
   <si>
@@ -395,6 +392,60 @@
   </si>
   <si>
     <t>Create different messages for student professor in ics email</t>
+  </si>
+  <si>
+    <t>Complete Team Report</t>
+  </si>
+  <si>
+    <t>Sunday</t>
+  </si>
+  <si>
+    <t>Integrate CAFÉ data and login into webapp</t>
+  </si>
+  <si>
+    <t>Integrate Appointment database with webapp</t>
+  </si>
+  <si>
+    <t>unable to get into the database</t>
+  </si>
+  <si>
+    <t>Duffin?</t>
+  </si>
+  <si>
+    <t>Done; Abandoned</t>
+  </si>
+  <si>
+    <t>Moved to Sprint 4</t>
+  </si>
+  <si>
+    <t>50%; Moved to Sprint 4</t>
+  </si>
+  <si>
+    <t>On hold</t>
+  </si>
+  <si>
+    <t>5 - 4.8</t>
+  </si>
+  <si>
+    <t>6 - 4.9</t>
+  </si>
+  <si>
+    <t>7 - 4.1</t>
+  </si>
+  <si>
+    <t>8 - 4.11</t>
+  </si>
+  <si>
+    <t>Integrate ics/email with webapp</t>
+  </si>
+  <si>
+    <t>Schedule stakeholder meeting</t>
+  </si>
+  <si>
+    <t>All, Jimmy</t>
+  </si>
+  <si>
+    <t>30%; pushed to Sprint 4</t>
   </si>
 </sst>
 </file>
@@ -509,7 +560,7 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="56">
+  <cellXfs count="58">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -637,6 +688,8 @@
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -998,10 +1051,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G101"/>
+  <dimension ref="A1:G104"/>
   <sheetViews>
-    <sheetView tabSelected="1" showRuler="0" topLeftCell="A60" zoomScale="78" zoomScaleNormal="78" workbookViewId="0">
-      <selection activeCell="F81" sqref="F81"/>
+    <sheetView tabSelected="1" showRuler="0" topLeftCell="A79" zoomScale="78" zoomScaleNormal="78" workbookViewId="0">
+      <selection activeCell="F95" sqref="F95"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.125" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -1021,11 +1074,11 @@
       <c r="B1" s="21" t="s">
         <v>32</v>
       </c>
-      <c r="C1" s="49" t="s">
+      <c r="C1" s="51" t="s">
         <v>37</v>
       </c>
-      <c r="D1" s="49"/>
-      <c r="E1" s="49"/>
+      <c r="D1" s="51"/>
+      <c r="E1" s="51"/>
       <c r="F1" s="20" t="s">
         <v>34</v>
       </c>
@@ -1035,14 +1088,14 @@
       <c r="B2" s="20" t="s">
         <v>33</v>
       </c>
-      <c r="C2" s="50"/>
-      <c r="D2" s="50"/>
-      <c r="E2" s="50"/>
+      <c r="C2" s="52"/>
+      <c r="D2" s="52"/>
+      <c r="E2" s="52"/>
       <c r="F2" s="20"/>
     </row>
     <row r="3" spans="1:7" ht="18" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A3" s="20"/>
-      <c r="B3" s="51"/>
+      <c r="B3" s="53"/>
       <c r="C3" s="23" t="s">
         <v>24</v>
       </c>
@@ -1054,7 +1107,7 @@
     </row>
     <row r="4" spans="1:7" ht="18" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A4" s="20"/>
-      <c r="B4" s="51"/>
+      <c r="B4" s="53"/>
       <c r="C4" s="22" t="s">
         <v>27</v>
       </c>
@@ -1066,7 +1119,7 @@
     </row>
     <row r="5" spans="1:7" ht="18" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A5" s="20"/>
-      <c r="B5" s="51"/>
+      <c r="B5" s="53"/>
       <c r="C5" s="22" t="s">
         <v>28</v>
       </c>
@@ -1078,7 +1131,7 @@
     </row>
     <row r="6" spans="1:7" ht="18" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A6" s="20"/>
-      <c r="B6" s="51"/>
+      <c r="B6" s="53"/>
       <c r="C6" s="22" t="s">
         <v>23</v>
       </c>
@@ -1090,7 +1143,7 @@
     </row>
     <row r="7" spans="1:7" ht="18" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A7" s="2"/>
-      <c r="B7" s="51"/>
+      <c r="B7" s="53"/>
       <c r="C7" s="40" t="s">
         <v>78</v>
       </c>
@@ -1140,8 +1193,8 @@
       <c r="E10" s="3" t="s">
         <v>66</v>
       </c>
-      <c r="F10" s="54"/>
-      <c r="G10" s="54"/>
+      <c r="F10" s="56"/>
+      <c r="G10" s="56"/>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A11" s="1">
@@ -1159,10 +1212,10 @@
       <c r="E11" s="3" t="s">
         <v>65</v>
       </c>
-      <c r="F11" s="55" t="s">
+      <c r="F11" s="57" t="s">
         <v>73</v>
       </c>
-      <c r="G11" s="55"/>
+      <c r="G11" s="57"/>
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A12" s="1">
@@ -1178,8 +1231,8 @@
         <v>42486</v>
       </c>
       <c r="E12" s="12"/>
-      <c r="F12" s="54"/>
-      <c r="G12" s="54"/>
+      <c r="F12" s="56"/>
+      <c r="G12" s="56"/>
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A13" s="1">
@@ -1195,8 +1248,8 @@
         <v>42493</v>
       </c>
       <c r="E13" s="12"/>
-      <c r="F13" s="54"/>
-      <c r="G13" s="54"/>
+      <c r="F13" s="56"/>
+      <c r="G13" s="56"/>
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A14" s="1"/>
@@ -1204,8 +1257,8 @@
       <c r="C14" s="16"/>
       <c r="D14" s="16"/>
       <c r="E14" s="12"/>
-      <c r="F14" s="54"/>
-      <c r="G14" s="54"/>
+      <c r="F14" s="56"/>
+      <c r="G14" s="56"/>
     </row>
     <row r="15" spans="1:7" ht="15.6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A15" s="2"/>
@@ -1287,7 +1340,7 @@
         <v>117</v>
       </c>
       <c r="F19" s="1" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="G19" s="1"/>
     </row>
@@ -1306,7 +1359,7 @@
         <v>65</v>
       </c>
       <c r="F20" s="1" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="G20" s="1"/>
     </row>
@@ -1325,7 +1378,7 @@
         <v>65</v>
       </c>
       <c r="F21" s="1" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="G21" s="1"/>
     </row>
@@ -1344,7 +1397,7 @@
         <v>65</v>
       </c>
       <c r="F22" s="1" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="G22" s="1"/>
     </row>
@@ -1597,8 +1650,8 @@
       <c r="F40" s="13"/>
     </row>
     <row r="41" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="B41" s="52"/>
-      <c r="C41" s="53"/>
+      <c r="B41" s="54"/>
+      <c r="C41" s="55"/>
       <c r="F41" s="13"/>
       <c r="G41" s="13"/>
     </row>
@@ -1979,9 +2032,11 @@
         <v>85</v>
       </c>
       <c r="E63" s="1" t="s">
-        <v>65</v>
-      </c>
-      <c r="F63" s="13"/>
+        <v>141</v>
+      </c>
+      <c r="F63" s="13" t="s">
+        <v>128</v>
+      </c>
     </row>
     <row r="64" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A64" s="1">
@@ -1996,10 +2051,10 @@
       <c r="D64" s="1" t="s">
         <v>61</v>
       </c>
-      <c r="E64" s="1"/>
-      <c r="F64" s="13" t="s">
-        <v>118</v>
-      </c>
+      <c r="E64" s="1" t="s">
+        <v>76</v>
+      </c>
+      <c r="F64" s="13"/>
     </row>
     <row r="65" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A65" s="1">
@@ -2014,10 +2069,10 @@
       <c r="D65" s="1" t="s">
         <v>61</v>
       </c>
-      <c r="E65" s="1"/>
-      <c r="F65" s="13" t="s">
-        <v>118</v>
-      </c>
+      <c r="E65" s="1" t="s">
+        <v>76</v>
+      </c>
+      <c r="F65" s="13"/>
     </row>
     <row r="66" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A66" s="1">
@@ -2033,7 +2088,7 @@
         <v>89</v>
       </c>
       <c r="E66" s="1" t="s">
-        <v>76</v>
+        <v>132</v>
       </c>
       <c r="F66" s="13"/>
     </row>
@@ -2069,7 +2124,7 @@
         <v>92</v>
       </c>
       <c r="E68" s="1" t="s">
-        <v>65</v>
+        <v>76</v>
       </c>
       <c r="F68" s="13"/>
     </row>
@@ -2085,7 +2140,7 @@
         <v>94</v>
       </c>
       <c r="E69" s="1" t="s">
-        <v>65</v>
+        <v>131</v>
       </c>
       <c r="F69" s="13"/>
     </row>
@@ -2102,9 +2157,14 @@
       <c r="D70" s="1" t="s">
         <v>96</v>
       </c>
-      <c r="E70" s="1"/>
+      <c r="E70" s="1" t="s">
+        <v>133</v>
+      </c>
       <c r="F70" s="13" t="s">
-        <v>118</v>
+        <v>128</v>
+      </c>
+      <c r="G70" s="1" t="s">
+        <v>129</v>
       </c>
     </row>
     <row r="71" spans="1:7" s="43" customFormat="1" x14ac:dyDescent="0.25">
@@ -2118,9 +2178,14 @@
       <c r="D71" s="1" t="s">
         <v>96</v>
       </c>
-      <c r="E71" s="1"/>
+      <c r="E71" s="1" t="s">
+        <v>133</v>
+      </c>
       <c r="F71" s="13" t="s">
-        <v>118</v>
+        <v>128</v>
+      </c>
+      <c r="G71" s="1" t="s">
+        <v>129</v>
       </c>
     </row>
     <row r="72" spans="1:7" s="43" customFormat="1" x14ac:dyDescent="0.25">
@@ -2136,9 +2201,11 @@
       <c r="D72" s="1" t="s">
         <v>99</v>
       </c>
-      <c r="E72" s="1"/>
+      <c r="E72" s="1" t="s">
+        <v>133</v>
+      </c>
       <c r="F72" s="13" t="s">
-        <v>118</v>
+        <v>128</v>
       </c>
     </row>
     <row r="73" spans="1:7" s="43" customFormat="1" ht="31.5" x14ac:dyDescent="0.25">
@@ -2154,9 +2221,11 @@
       <c r="D73" s="1" t="s">
         <v>99</v>
       </c>
-      <c r="E73" s="1"/>
+      <c r="E73" s="1" t="s">
+        <v>133</v>
+      </c>
       <c r="F73" s="13" t="s">
-        <v>118</v>
+        <v>128</v>
       </c>
     </row>
     <row r="74" spans="1:7" s="43" customFormat="1" x14ac:dyDescent="0.25">
@@ -2188,8 +2257,8 @@
       <c r="D75" s="1" t="s">
         <v>64</v>
       </c>
-      <c r="E75" s="48">
-        <v>0.4</v>
+      <c r="E75" s="48" t="s">
+        <v>76</v>
       </c>
       <c r="F75" s="13"/>
     </row>
@@ -2198,7 +2267,7 @@
         <v>14</v>
       </c>
       <c r="B76" s="13" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="C76" s="1">
         <v>5</v>
@@ -2206,8 +2275,8 @@
       <c r="D76" s="1" t="s">
         <v>103</v>
       </c>
-      <c r="E76" s="48">
-        <v>0.4</v>
+      <c r="E76" s="48" t="s">
+        <v>76</v>
       </c>
       <c r="F76" s="13"/>
     </row>
@@ -2240,10 +2309,10 @@
         <v>5</v>
       </c>
       <c r="D78" s="1" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="E78" s="1" t="s">
-        <v>65</v>
+        <v>76</v>
       </c>
       <c r="F78" s="13"/>
     </row>
@@ -2260,8 +2329,8 @@
       <c r="D79" s="11" t="s">
         <v>64</v>
       </c>
-      <c r="E79" s="41">
-        <v>0.5</v>
+      <c r="E79" s="41" t="s">
+        <v>130</v>
       </c>
       <c r="F79" s="11"/>
       <c r="G79" s="45"/>
@@ -2317,8 +2386,8 @@
       <c r="D82" s="5" t="s">
         <v>51</v>
       </c>
-      <c r="E82" s="41">
-        <v>0.8</v>
+      <c r="E82" s="41" t="s">
+        <v>76</v>
       </c>
       <c r="F82" s="45" t="s">
         <v>75</v>
@@ -2329,7 +2398,7 @@
         <v>19</v>
       </c>
       <c r="B83" s="34" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="C83" s="15">
         <v>1</v>
@@ -2385,108 +2454,250 @@
       <c r="A87" s="1">
         <v>1</v>
       </c>
+      <c r="B87" s="13" t="s">
+        <v>124</v>
+      </c>
       <c r="C87" s="1"/>
-      <c r="D87" s="43"/>
-      <c r="E87" s="43"/>
+      <c r="D87" s="1" t="s">
+        <v>71</v>
+      </c>
+      <c r="E87" s="41" t="s">
+        <v>65</v>
+      </c>
+      <c r="F87" t="s">
+        <v>125</v>
+      </c>
     </row>
     <row r="88" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A88" s="1">
         <v>2</v>
       </c>
+      <c r="B88" s="13" t="s">
+        <v>138</v>
+      </c>
       <c r="C88" s="1"/>
-      <c r="D88" s="43"/>
-      <c r="E88" s="43"/>
+      <c r="D88" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="E88" s="41" t="s">
+        <v>65</v>
+      </c>
     </row>
     <row r="89" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A89" s="1">
         <v>3</v>
       </c>
+      <c r="B89" s="13" t="s">
+        <v>126</v>
+      </c>
       <c r="C89" s="1"/>
-      <c r="D89" s="43"/>
-      <c r="E89" s="43"/>
+      <c r="D89" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="E89" s="41" t="s">
+        <v>65</v>
+      </c>
     </row>
     <row r="90" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A90" s="1">
         <v>4</v>
       </c>
+      <c r="B90" s="13" t="s">
+        <v>127</v>
+      </c>
       <c r="C90" s="1"/>
-      <c r="D90" s="43"/>
-      <c r="E90" s="43"/>
-    </row>
-    <row r="91" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A91" s="1">
+      <c r="D90" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="E90" s="41" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="91" spans="1:7" s="49" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A91" s="1" t="s">
+        <v>134</v>
+      </c>
+      <c r="B91" s="13" t="s">
+        <v>95</v>
+      </c>
+      <c r="C91" s="1" t="s">
+        <v>112</v>
+      </c>
+      <c r="D91" s="1" t="s">
+        <v>96</v>
+      </c>
+      <c r="E91" s="1" t="s">
+        <v>133</v>
+      </c>
+      <c r="F91" s="13" t="s">
+        <v>128</v>
+      </c>
+      <c r="G91" s="1" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="92" spans="1:7" s="49" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A92" s="1" t="s">
+        <v>135</v>
+      </c>
+      <c r="B92" s="13" t="s">
+        <v>97</v>
+      </c>
+      <c r="C92" s="1"/>
+      <c r="D92" s="1" t="s">
+        <v>96</v>
+      </c>
+      <c r="E92" s="1" t="s">
+        <v>133</v>
+      </c>
+      <c r="F92" s="13" t="s">
+        <v>128</v>
+      </c>
+      <c r="G92" s="1" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="93" spans="1:7" s="49" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A93" s="1" t="s">
+        <v>136</v>
+      </c>
+      <c r="B93" s="13" t="s">
+        <v>98</v>
+      </c>
+      <c r="C93" s="1" t="s">
+        <v>112</v>
+      </c>
+      <c r="D93" s="1" t="s">
+        <v>99</v>
+      </c>
+      <c r="E93" s="1" t="s">
+        <v>133</v>
+      </c>
+      <c r="F93" s="13" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="94" spans="1:7" s="49" customFormat="1" ht="31.5" x14ac:dyDescent="0.25">
+      <c r="A94" s="1" t="s">
+        <v>137</v>
+      </c>
+      <c r="B94" s="13" t="s">
+        <v>100</v>
+      </c>
+      <c r="C94" s="1" t="s">
+        <v>112</v>
+      </c>
+      <c r="D94" s="1" t="s">
+        <v>99</v>
+      </c>
+      <c r="E94" s="1" t="s">
+        <v>133</v>
+      </c>
+      <c r="F94" s="13" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="95" spans="1:7" s="49" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A95" s="1">
+        <v>9</v>
+      </c>
+      <c r="B95" s="13" t="s">
+        <v>139</v>
+      </c>
+      <c r="C95" s="1"/>
+      <c r="D95" s="1" t="s">
+        <v>140</v>
+      </c>
+      <c r="E95" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="F95" s="13"/>
+    </row>
+    <row r="96" spans="1:7" s="50" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A96" s="1">
+        <v>1</v>
+      </c>
+      <c r="B96" s="13" t="s">
+        <v>84</v>
+      </c>
+      <c r="C96" s="1">
+        <v>6</v>
+      </c>
+      <c r="D96" s="1" t="s">
+        <v>85</v>
+      </c>
+      <c r="E96" s="48">
+        <v>0.3</v>
+      </c>
+      <c r="F96" s="13" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="97" spans="1:7" s="49" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A97" s="1"/>
+      <c r="B97" s="13"/>
+      <c r="C97" s="1"/>
+      <c r="D97" s="1"/>
+      <c r="E97" s="1"/>
+      <c r="F97" s="13"/>
+    </row>
+    <row r="98" spans="1:7" ht="20.25" x14ac:dyDescent="0.3">
+      <c r="B98" s="17" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="99" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A99" s="7" t="s">
+        <v>1</v>
+      </c>
+      <c r="B99" s="14" t="s">
+        <v>15</v>
+      </c>
+      <c r="C99" s="7" t="s">
+        <v>21</v>
+      </c>
+      <c r="D99" s="7" t="s">
+        <v>9</v>
+      </c>
+      <c r="E99" s="7" t="s">
+        <v>10</v>
+      </c>
+      <c r="F99" s="7" t="s">
+        <v>13</v>
+      </c>
+      <c r="G99" s="7" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="100" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A100" s="1">
+        <v>1</v>
+      </c>
+      <c r="C100" s="1"/>
+    </row>
+    <row r="101" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A101" s="1">
+        <v>2</v>
+      </c>
+      <c r="C101" s="1"/>
+    </row>
+    <row r="102" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A102" s="1">
+        <v>3</v>
+      </c>
+      <c r="C102" s="1"/>
+    </row>
+    <row r="103" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A103" s="1">
+        <v>4</v>
+      </c>
+      <c r="C103" s="1"/>
+    </row>
+    <row r="104" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A104" s="1">
         <v>5</v>
       </c>
-      <c r="C91" s="1"/>
-      <c r="D91" s="43"/>
-      <c r="E91" s="43"/>
-    </row>
-    <row r="92" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="C92" s="1"/>
-    </row>
-    <row r="93" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="C93" s="1"/>
-    </row>
-    <row r="94" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="C94" s="1"/>
-    </row>
-    <row r="95" spans="1:7" ht="20.25" x14ac:dyDescent="0.3">
-      <c r="B95" s="17" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="96" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A96" s="7" t="s">
-        <v>1</v>
-      </c>
-      <c r="B96" s="14" t="s">
-        <v>15</v>
-      </c>
-      <c r="C96" s="7" t="s">
-        <v>21</v>
-      </c>
-      <c r="D96" s="7" t="s">
-        <v>9</v>
-      </c>
-      <c r="E96" s="7" t="s">
-        <v>10</v>
-      </c>
-      <c r="F96" s="7" t="s">
-        <v>13</v>
-      </c>
-      <c r="G96" s="7" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="97" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A97" s="1">
-        <v>1</v>
-      </c>
-      <c r="C97" s="1"/>
-    </row>
-    <row r="98" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A98" s="1">
-        <v>2</v>
-      </c>
-      <c r="C98" s="1"/>
-    </row>
-    <row r="99" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A99" s="1">
-        <v>3</v>
-      </c>
-      <c r="C99" s="1"/>
-    </row>
-    <row r="100" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A100" s="1">
-        <v>4</v>
-      </c>
-      <c r="C100" s="1"/>
-    </row>
-    <row r="101" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A101" s="1">
-        <v>5</v>
-      </c>
-      <c r="C101" s="1"/>
+      <c r="C104" s="1"/>
     </row>
   </sheetData>
   <mergeCells count="9">

</xml_diff>

<commit_message>
updated backlog due to typo in intial version
</commit_message>
<xml_diff>
--- a/Documentation/backlogs/masterProductBacklog.xlsx
+++ b/Documentation/backlogs/masterProductBacklog.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="294" uniqueCount="142">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="319" uniqueCount="149">
   <si>
     <t>Sprints</t>
   </si>
@@ -370,21 +370,12 @@
     <t>4,6</t>
   </si>
   <si>
-    <t>waiting</t>
-  </si>
-  <si>
     <t>In Progress (75%)</t>
   </si>
   <si>
-    <t>In Progress (90%)</t>
-  </si>
-  <si>
     <t>In Progress (70%)</t>
   </si>
   <si>
-    <t>In Progress (85%)</t>
-  </si>
-  <si>
     <t xml:space="preserve">     hashing/security for passwords</t>
   </si>
   <si>
@@ -446,6 +437,36 @@
   </si>
   <si>
     <t>30%; pushed to Sprint 4</t>
+  </si>
+  <si>
+    <t>In Progress; On hold</t>
+  </si>
+  <si>
+    <t>30%; In progress</t>
+  </si>
+  <si>
+    <t>Integration of Components (added 4-26-16)</t>
+  </si>
+  <si>
+    <t>In Progress (10%)</t>
+  </si>
+  <si>
+    <t>Waiting</t>
+  </si>
+  <si>
+    <t>4,8</t>
+  </si>
+  <si>
+    <t>8, 1</t>
+  </si>
+  <si>
+    <t>* General Documentation *</t>
+  </si>
+  <si>
+    <t>10 - 4.1</t>
+  </si>
+  <si>
+    <t>Create landing page after submission in GUI</t>
   </si>
 </sst>
 </file>
@@ -560,7 +581,7 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="58">
+  <cellXfs count="59">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -688,6 +709,7 @@
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
@@ -1051,10 +1073,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G104"/>
+  <dimension ref="A1:G105"/>
   <sheetViews>
-    <sheetView tabSelected="1" showRuler="0" topLeftCell="A79" zoomScale="78" zoomScaleNormal="78" workbookViewId="0">
-      <selection activeCell="F95" sqref="F95"/>
+    <sheetView tabSelected="1" showRuler="0" zoomScale="78" zoomScaleNormal="78" workbookViewId="0">
+      <selection activeCell="E103" sqref="E103"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.125" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -1074,11 +1096,11 @@
       <c r="B1" s="21" t="s">
         <v>32</v>
       </c>
-      <c r="C1" s="51" t="s">
+      <c r="C1" s="52" t="s">
         <v>37</v>
       </c>
-      <c r="D1" s="51"/>
-      <c r="E1" s="51"/>
+      <c r="D1" s="52"/>
+      <c r="E1" s="52"/>
       <c r="F1" s="20" t="s">
         <v>34</v>
       </c>
@@ -1088,14 +1110,14 @@
       <c r="B2" s="20" t="s">
         <v>33</v>
       </c>
-      <c r="C2" s="52"/>
-      <c r="D2" s="52"/>
-      <c r="E2" s="52"/>
+      <c r="C2" s="53"/>
+      <c r="D2" s="53"/>
+      <c r="E2" s="53"/>
       <c r="F2" s="20"/>
     </row>
     <row r="3" spans="1:7" ht="18" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A3" s="20"/>
-      <c r="B3" s="53"/>
+      <c r="B3" s="54"/>
       <c r="C3" s="23" t="s">
         <v>24</v>
       </c>
@@ -1107,48 +1129,48 @@
     </row>
     <row r="4" spans="1:7" ht="18" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A4" s="20"/>
-      <c r="B4" s="53"/>
+      <c r="B4" s="54"/>
       <c r="C4" s="22" t="s">
         <v>27</v>
       </c>
       <c r="D4" s="24">
-        <v>42463</v>
+        <v>42486</v>
       </c>
       <c r="E4" s="22"/>
       <c r="F4" s="20"/>
     </row>
     <row r="5" spans="1:7" ht="18" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A5" s="20"/>
-      <c r="B5" s="53"/>
+      <c r="B5" s="54"/>
       <c r="C5" s="22" t="s">
         <v>28</v>
       </c>
       <c r="D5" s="24">
-        <v>42463</v>
+        <v>42486</v>
       </c>
       <c r="E5" s="22"/>
       <c r="F5" s="20"/>
     </row>
     <row r="6" spans="1:7" ht="18" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A6" s="20"/>
-      <c r="B6" s="53"/>
+      <c r="B6" s="54"/>
       <c r="C6" s="22" t="s">
         <v>23</v>
       </c>
       <c r="D6" s="24">
-        <v>42481</v>
+        <v>42488</v>
       </c>
       <c r="E6" s="22"/>
       <c r="F6" s="20"/>
     </row>
     <row r="7" spans="1:7" ht="18" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A7" s="2"/>
-      <c r="B7" s="53"/>
+      <c r="B7" s="54"/>
       <c r="C7" s="40" t="s">
         <v>78</v>
       </c>
       <c r="D7" s="24">
-        <v>42481</v>
+        <v>42488</v>
       </c>
       <c r="E7" s="42"/>
     </row>
@@ -1193,8 +1215,8 @@
       <c r="E10" s="3" t="s">
         <v>66</v>
       </c>
-      <c r="F10" s="56"/>
-      <c r="G10" s="56"/>
+      <c r="F10" s="57"/>
+      <c r="G10" s="57"/>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A11" s="1">
@@ -1210,12 +1232,12 @@
         <v>42479</v>
       </c>
       <c r="E11" s="3" t="s">
-        <v>65</v>
-      </c>
-      <c r="F11" s="57" t="s">
+        <v>66</v>
+      </c>
+      <c r="F11" s="58" t="s">
         <v>73</v>
       </c>
-      <c r="G11" s="57"/>
+      <c r="G11" s="58"/>
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A12" s="1">
@@ -1230,9 +1252,11 @@
       <c r="D12" s="16">
         <v>42486</v>
       </c>
-      <c r="E12" s="12"/>
-      <c r="F12" s="56"/>
-      <c r="G12" s="56"/>
+      <c r="E12" s="12" t="s">
+        <v>66</v>
+      </c>
+      <c r="F12" s="57"/>
+      <c r="G12" s="57"/>
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A13" s="1">
@@ -1247,9 +1271,11 @@
       <c r="D13" s="16">
         <v>42493</v>
       </c>
-      <c r="E13" s="12"/>
-      <c r="F13" s="56"/>
-      <c r="G13" s="56"/>
+      <c r="E13" s="12" t="s">
+        <v>65</v>
+      </c>
+      <c r="F13" s="57"/>
+      <c r="G13" s="57"/>
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A14" s="1"/>
@@ -1257,8 +1283,8 @@
       <c r="C14" s="16"/>
       <c r="D14" s="16"/>
       <c r="E14" s="12"/>
-      <c r="F14" s="56"/>
-      <c r="G14" s="56"/>
+      <c r="F14" s="57"/>
+      <c r="G14" s="57"/>
     </row>
     <row r="15" spans="1:7" ht="15.6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A15" s="2"/>
@@ -1318,12 +1344,14 @@
       </c>
       <c r="D18" s="1"/>
       <c r="E18" s="1" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="F18" s="1" t="s">
         <v>65</v>
       </c>
-      <c r="G18" s="1"/>
+      <c r="G18" s="1" t="s">
+        <v>65</v>
+      </c>
     </row>
     <row r="19" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A19" s="1">
@@ -1337,12 +1365,14 @@
       </c>
       <c r="D19" s="1"/>
       <c r="E19" s="1" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="F19" s="1" t="s">
-        <v>118</v>
-      </c>
-      <c r="G19" s="1"/>
+        <v>76</v>
+      </c>
+      <c r="G19" s="1" t="s">
+        <v>76</v>
+      </c>
     </row>
     <row r="20" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A20" s="25">
@@ -1359,9 +1389,11 @@
         <v>65</v>
       </c>
       <c r="F20" s="1" t="s">
-        <v>119</v>
-      </c>
-      <c r="G20" s="1"/>
+        <v>117</v>
+      </c>
+      <c r="G20" s="1" t="s">
+        <v>117</v>
+      </c>
     </row>
     <row r="21" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A21" s="25">
@@ -1378,9 +1410,11 @@
         <v>65</v>
       </c>
       <c r="F21" s="1" t="s">
-        <v>119</v>
-      </c>
-      <c r="G21" s="1"/>
+        <v>117</v>
+      </c>
+      <c r="G21" s="1" t="s">
+        <v>117</v>
+      </c>
     </row>
     <row r="22" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A22" s="25">
@@ -1397,9 +1431,11 @@
         <v>65</v>
       </c>
       <c r="F22" s="1" t="s">
-        <v>120</v>
-      </c>
-      <c r="G22" s="1"/>
+        <v>76</v>
+      </c>
+      <c r="G22" s="1" t="s">
+        <v>76</v>
+      </c>
     </row>
     <row r="23" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A23" s="25">
@@ -1413,12 +1449,14 @@
       </c>
       <c r="D23" s="25"/>
       <c r="E23" s="1" t="s">
-        <v>116</v>
+        <v>143</v>
       </c>
       <c r="F23" s="1" t="s">
-        <v>65</v>
-      </c>
-      <c r="G23" s="1"/>
+        <v>76</v>
+      </c>
+      <c r="G23" s="1" t="s">
+        <v>76</v>
+      </c>
     </row>
     <row r="24" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A24" s="25">
@@ -1437,7 +1475,9 @@
       <c r="F24" s="1" t="s">
         <v>76</v>
       </c>
-      <c r="G24" s="1"/>
+      <c r="G24" s="1" t="s">
+        <v>76</v>
+      </c>
     </row>
     <row r="25" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A25" s="25">
@@ -1454,27 +1494,43 @@
         <v>65</v>
       </c>
       <c r="F25" s="1" t="s">
-        <v>65</v>
-      </c>
-      <c r="G25" s="1"/>
+        <v>76</v>
+      </c>
+      <c r="G25" s="1" t="s">
+        <v>76</v>
+      </c>
     </row>
     <row r="26" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A26" s="25">
         <v>8</v>
       </c>
-      <c r="B26" s="10"/>
-      <c r="C26" s="1"/>
+      <c r="B26" s="10" t="s">
+        <v>141</v>
+      </c>
+      <c r="C26" s="1">
+        <v>1</v>
+      </c>
       <c r="D26" s="10"/>
-      <c r="E26" s="3"/>
-      <c r="F26" s="26"/>
-      <c r="G26" s="1"/>
+      <c r="E26" s="1" t="s">
+        <v>143</v>
+      </c>
+      <c r="F26" s="26" t="s">
+        <v>142</v>
+      </c>
+      <c r="G26" s="1" t="s">
+        <v>65</v>
+      </c>
     </row>
     <row r="27" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A27" s="25">
         <v>9</v>
       </c>
-      <c r="B27" s="10"/>
-      <c r="C27" s="1"/>
+      <c r="B27" s="10" t="s">
+        <v>146</v>
+      </c>
+      <c r="C27" s="1" t="s">
+        <v>70</v>
+      </c>
       <c r="D27" s="1"/>
       <c r="E27" s="3"/>
       <c r="F27" s="26"/>
@@ -1650,8 +1706,8 @@
       <c r="F40" s="13"/>
     </row>
     <row r="41" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="B41" s="54"/>
-      <c r="C41" s="55"/>
+      <c r="B41" s="55"/>
+      <c r="C41" s="56"/>
       <c r="F41" s="13"/>
       <c r="G41" s="13"/>
     </row>
@@ -2032,10 +2088,10 @@
         <v>85</v>
       </c>
       <c r="E63" s="1" t="s">
-        <v>141</v>
+        <v>138</v>
       </c>
       <c r="F63" s="13" t="s">
-        <v>128</v>
+        <v>125</v>
       </c>
     </row>
     <row r="64" spans="1:7" x14ac:dyDescent="0.25">
@@ -2088,7 +2144,7 @@
         <v>89</v>
       </c>
       <c r="E66" s="1" t="s">
-        <v>132</v>
+        <v>129</v>
       </c>
       <c r="F66" s="13"/>
     </row>
@@ -2140,7 +2196,7 @@
         <v>94</v>
       </c>
       <c r="E69" s="1" t="s">
-        <v>131</v>
+        <v>128</v>
       </c>
       <c r="F69" s="13"/>
     </row>
@@ -2158,13 +2214,13 @@
         <v>96</v>
       </c>
       <c r="E70" s="1" t="s">
-        <v>133</v>
+        <v>130</v>
       </c>
       <c r="F70" s="13" t="s">
-        <v>128</v>
+        <v>125</v>
       </c>
       <c r="G70" s="1" t="s">
-        <v>129</v>
+        <v>126</v>
       </c>
     </row>
     <row r="71" spans="1:7" s="43" customFormat="1" x14ac:dyDescent="0.25">
@@ -2179,13 +2235,13 @@
         <v>96</v>
       </c>
       <c r="E71" s="1" t="s">
-        <v>133</v>
+        <v>130</v>
       </c>
       <c r="F71" s="13" t="s">
-        <v>128</v>
+        <v>125</v>
       </c>
       <c r="G71" s="1" t="s">
-        <v>129</v>
+        <v>126</v>
       </c>
     </row>
     <row r="72" spans="1:7" s="43" customFormat="1" x14ac:dyDescent="0.25">
@@ -2202,10 +2258,10 @@
         <v>99</v>
       </c>
       <c r="E72" s="1" t="s">
-        <v>133</v>
+        <v>130</v>
       </c>
       <c r="F72" s="13" t="s">
-        <v>128</v>
+        <v>125</v>
       </c>
     </row>
     <row r="73" spans="1:7" s="43" customFormat="1" ht="31.5" x14ac:dyDescent="0.25">
@@ -2222,10 +2278,10 @@
         <v>99</v>
       </c>
       <c r="E73" s="1" t="s">
-        <v>133</v>
+        <v>130</v>
       </c>
       <c r="F73" s="13" t="s">
-        <v>128</v>
+        <v>125</v>
       </c>
     </row>
     <row r="74" spans="1:7" s="43" customFormat="1" x14ac:dyDescent="0.25">
@@ -2267,7 +2323,7 @@
         <v>14</v>
       </c>
       <c r="B76" s="13" t="s">
-        <v>121</v>
+        <v>118</v>
       </c>
       <c r="C76" s="1">
         <v>5</v>
@@ -2309,7 +2365,7 @@
         <v>5</v>
       </c>
       <c r="D78" s="1" t="s">
-        <v>122</v>
+        <v>119</v>
       </c>
       <c r="E78" s="1" t="s">
         <v>76</v>
@@ -2330,7 +2386,7 @@
         <v>64</v>
       </c>
       <c r="E79" s="41" t="s">
-        <v>130</v>
+        <v>127</v>
       </c>
       <c r="F79" s="11"/>
       <c r="G79" s="45"/>
@@ -2398,7 +2454,7 @@
         <v>19</v>
       </c>
       <c r="B83" s="34" t="s">
-        <v>123</v>
+        <v>120</v>
       </c>
       <c r="C83" s="15">
         <v>1</v>
@@ -2455,9 +2511,11 @@
         <v>1</v>
       </c>
       <c r="B87" s="13" t="s">
-        <v>124</v>
-      </c>
-      <c r="C87" s="1"/>
+        <v>121</v>
+      </c>
+      <c r="C87" s="1" t="s">
+        <v>70</v>
+      </c>
       <c r="D87" s="1" t="s">
         <v>71</v>
       </c>
@@ -2465,7 +2523,7 @@
         <v>65</v>
       </c>
       <c r="F87" t="s">
-        <v>125</v>
+        <v>122</v>
       </c>
     </row>
     <row r="88" spans="1:7" x14ac:dyDescent="0.25">
@@ -2473,9 +2531,11 @@
         <v>2</v>
       </c>
       <c r="B88" s="13" t="s">
-        <v>138</v>
-      </c>
-      <c r="C88" s="1"/>
+        <v>135</v>
+      </c>
+      <c r="C88" s="1" t="s">
+        <v>145</v>
+      </c>
       <c r="D88" s="1" t="s">
         <v>58</v>
       </c>
@@ -2488,9 +2548,11 @@
         <v>3</v>
       </c>
       <c r="B89" s="13" t="s">
-        <v>126</v>
-      </c>
-      <c r="C89" s="1"/>
+        <v>123</v>
+      </c>
+      <c r="C89" s="1">
+        <v>8</v>
+      </c>
       <c r="D89" s="1" t="s">
         <v>64</v>
       </c>
@@ -2503,9 +2565,11 @@
         <v>4</v>
       </c>
       <c r="B90" s="13" t="s">
-        <v>127</v>
-      </c>
-      <c r="C90" s="1"/>
+        <v>124</v>
+      </c>
+      <c r="C90" s="1">
+        <v>8</v>
+      </c>
       <c r="D90" s="1" t="s">
         <v>51</v>
       </c>
@@ -2515,7 +2579,7 @@
     </row>
     <row r="91" spans="1:7" s="49" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A91" s="1" t="s">
-        <v>134</v>
+        <v>131</v>
       </c>
       <c r="B91" s="13" t="s">
         <v>95</v>
@@ -2527,39 +2591,41 @@
         <v>96</v>
       </c>
       <c r="E91" s="1" t="s">
-        <v>133</v>
+        <v>139</v>
       </c>
       <c r="F91" s="13" t="s">
-        <v>128</v>
+        <v>125</v>
       </c>
       <c r="G91" s="1" t="s">
-        <v>129</v>
+        <v>126</v>
       </c>
     </row>
     <row r="92" spans="1:7" s="49" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A92" s="1" t="s">
-        <v>135</v>
+        <v>132</v>
       </c>
       <c r="B92" s="13" t="s">
         <v>97</v>
       </c>
-      <c r="C92" s="1"/>
+      <c r="C92" s="1" t="s">
+        <v>144</v>
+      </c>
       <c r="D92" s="1" t="s">
         <v>96</v>
       </c>
       <c r="E92" s="1" t="s">
-        <v>133</v>
+        <v>139</v>
       </c>
       <c r="F92" s="13" t="s">
-        <v>128</v>
+        <v>125</v>
       </c>
       <c r="G92" s="1" t="s">
-        <v>129</v>
+        <v>126</v>
       </c>
     </row>
     <row r="93" spans="1:7" s="49" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A93" s="1" t="s">
-        <v>136</v>
+        <v>133</v>
       </c>
       <c r="B93" s="13" t="s">
         <v>98</v>
@@ -2571,15 +2637,15 @@
         <v>99</v>
       </c>
       <c r="E93" s="1" t="s">
-        <v>133</v>
+        <v>139</v>
       </c>
       <c r="F93" s="13" t="s">
-        <v>128</v>
+        <v>125</v>
       </c>
     </row>
     <row r="94" spans="1:7" s="49" customFormat="1" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A94" s="1" t="s">
-        <v>137</v>
+        <v>134</v>
       </c>
       <c r="B94" s="13" t="s">
         <v>100</v>
@@ -2591,10 +2657,10 @@
         <v>99</v>
       </c>
       <c r="E94" s="1" t="s">
-        <v>133</v>
+        <v>139</v>
       </c>
       <c r="F94" s="13" t="s">
-        <v>128</v>
+        <v>125</v>
       </c>
     </row>
     <row r="95" spans="1:7" s="49" customFormat="1" x14ac:dyDescent="0.25">
@@ -2602,20 +2668,22 @@
         <v>9</v>
       </c>
       <c r="B95" s="13" t="s">
-        <v>139</v>
-      </c>
-      <c r="C95" s="1"/>
+        <v>136</v>
+      </c>
+      <c r="C95" s="1" t="s">
+        <v>70</v>
+      </c>
       <c r="D95" s="1" t="s">
-        <v>140</v>
+        <v>137</v>
       </c>
       <c r="E95" s="1" t="s">
         <v>65</v>
       </c>
       <c r="F95" s="13"/>
     </row>
-    <row r="96" spans="1:7" s="50" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A96" s="1">
-        <v>1</v>
+    <row r="96" spans="1:7" s="50" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A96" s="1" t="s">
+        <v>147</v>
       </c>
       <c r="B96" s="13" t="s">
         <v>84</v>
@@ -2626,78 +2694,96 @@
       <c r="D96" s="1" t="s">
         <v>85</v>
       </c>
-      <c r="E96" s="48">
-        <v>0.3</v>
+      <c r="E96" s="48" t="s">
+        <v>140</v>
       </c>
       <c r="F96" s="13" t="s">
-        <v>128</v>
+        <v>125</v>
       </c>
     </row>
     <row r="97" spans="1:7" s="49" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A97" s="1"/>
-      <c r="B97" s="13"/>
-      <c r="C97" s="1"/>
-      <c r="D97" s="1"/>
-      <c r="E97" s="1"/>
+      <c r="A97" s="1">
+        <v>11</v>
+      </c>
+      <c r="B97" s="13" t="s">
+        <v>148</v>
+      </c>
+      <c r="C97" s="1">
+        <v>0</v>
+      </c>
+      <c r="D97" s="1" t="s">
+        <v>94</v>
+      </c>
+      <c r="E97" s="1" t="s">
+        <v>65</v>
+      </c>
       <c r="F97" s="13"/>
     </row>
-    <row r="98" spans="1:7" ht="20.25" x14ac:dyDescent="0.3">
-      <c r="B98" s="17" t="s">
+    <row r="98" spans="1:7" s="51" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A98" s="1"/>
+      <c r="B98" s="13"/>
+      <c r="C98" s="1"/>
+      <c r="D98" s="1"/>
+      <c r="E98" s="1"/>
+      <c r="F98" s="13"/>
+    </row>
+    <row r="99" spans="1:7" ht="20.25" x14ac:dyDescent="0.3">
+      <c r="B99" s="17" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="99" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A99" s="7" t="s">
+    <row r="100" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A100" s="7" t="s">
         <v>1</v>
       </c>
-      <c r="B99" s="14" t="s">
+      <c r="B100" s="14" t="s">
         <v>15</v>
       </c>
-      <c r="C99" s="7" t="s">
+      <c r="C100" s="7" t="s">
         <v>21</v>
       </c>
-      <c r="D99" s="7" t="s">
+      <c r="D100" s="7" t="s">
         <v>9</v>
       </c>
-      <c r="E99" s="7" t="s">
+      <c r="E100" s="7" t="s">
         <v>10</v>
       </c>
-      <c r="F99" s="7" t="s">
+      <c r="F100" s="7" t="s">
         <v>13</v>
       </c>
-      <c r="G99" s="7" t="s">
+      <c r="G100" s="7" t="s">
         <v>22</v>
       </c>
-    </row>
-    <row r="100" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A100" s="1">
-        <v>1</v>
-      </c>
-      <c r="C100" s="1"/>
     </row>
     <row r="101" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A101" s="1">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C101" s="1"/>
     </row>
     <row r="102" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A102" s="1">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C102" s="1"/>
     </row>
     <row r="103" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A103" s="1">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="C103" s="1"/>
     </row>
     <row r="104" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A104" s="1">
+        <v>4</v>
+      </c>
+      <c r="C104" s="1"/>
+    </row>
+    <row r="105" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A105" s="1">
         <v>5</v>
       </c>
-      <c r="C104" s="1"/>
+      <c r="C105" s="1"/>
     </row>
   </sheetData>
   <mergeCells count="9">

</xml_diff>